<commit_message>
RE ordered and color coded reference sheet.
</commit_message>
<xml_diff>
--- a/src/resources/Fhir_Cohort_Import_Template.xlsx
+++ b/src/resources/Fhir_Cohort_Import_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\T21_Connectathon_Sets\Python_Generation\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB449184-A5EC-440E-B750-7E8F8FBF5295}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D05B9B-939D-479A-AE68-6BFCF811CBDC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1284" windowWidth="38400" windowHeight="21096" activeTab="1" xr2:uid="{B7CAF98F-F4CF-4673-A736-BDE9BA8D985C}"/>
+    <workbookView xWindow="-38400" yWindow="-1284" windowWidth="38400" windowHeight="21096" activeTab="3" xr2:uid="{B7CAF98F-F4CF-4673-A736-BDE9BA8D985C}"/>
   </bookViews>
   <sheets>
     <sheet name="ResourceDefinitions" sheetId="2" r:id="rId1"/>
@@ -321,7 +321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CK6" authorId="1" shapeId="0" xr:uid="{6DE12A49-1D75-498C-94E9-C5CC28C04B1A}">
+    <comment ref="CH6" authorId="1" shapeId="0" xr:uid="{6DE12A49-1D75-498C-94E9-C5CC28C04B1A}">
       <text>
         <r>
           <rPr>
@@ -338,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CL6" authorId="1" shapeId="0" xr:uid="{8B714178-3048-41FA-959C-3B69494C8BFA}">
+    <comment ref="CI6" authorId="1" shapeId="0" xr:uid="{8B714178-3048-41FA-959C-3B69494C8BFA}">
       <text>
         <r>
           <rPr>
@@ -355,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CM6" authorId="1" shapeId="0" xr:uid="{5BF9D6E7-0F8A-4170-9D07-CBF66A9C9F64}">
+    <comment ref="CJ6" authorId="1" shapeId="0" xr:uid="{5BF9D6E7-0F8A-4170-9D07-CBF66A9C9F64}">
       <text>
         <r>
           <rPr>
@@ -372,7 +372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CN6" authorId="1" shapeId="0" xr:uid="{9851491C-AC34-41E0-AB26-F9C66571CD3B}">
+    <comment ref="CK6" authorId="1" shapeId="0" xr:uid="{9851491C-AC34-41E0-AB26-F9C66571CD3B}">
       <text>
         <r>
           <rPr>
@@ -440,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CK7" authorId="3" shapeId="0" xr:uid="{19DD006D-3586-4D74-AC01-D724897B0F46}">
+    <comment ref="CH7" authorId="3" shapeId="0" xr:uid="{19DD006D-3586-4D74-AC01-D724897B0F46}">
       <text>
         <r>
           <rPr>
@@ -462,7 +462,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="287">
   <si>
     <t>Data Element</t>
   </si>
@@ -1321,6 +1321,9 @@
   </si>
   <si>
     <t>Device.type</t>
+  </si>
+  <si>
+    <t>Location.telecom.[0].use</t>
   </si>
 </sst>
 </file>
@@ -1371,7 +1374,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1390,8 +1393,110 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB691"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCB91"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFED91"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDFF91"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9EFF91"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF91FFD2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA1EFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA1C3FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFACA1FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9A1FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA1D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA1A1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCEA1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF8A1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9FFA1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA1FFAC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA1FFEF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1424,6 +1529,21 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1679,6 +1799,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1686,7 +1866,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1705,79 +1885,223 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1788,6 +2112,20 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFA1FFEF"/>
+      <color rgb="FFA1FFAC"/>
+      <color rgb="FFD9FFA1"/>
+      <color rgb="FFFFF8A1"/>
+      <color rgb="FFFFCEA1"/>
+      <color rgb="FFFFA1A1"/>
+      <color rgb="FFFFA1D9"/>
+      <color rgb="FFD9A1FF"/>
+      <color rgb="FFACA1FF"/>
+      <color rgb="FFA1C3FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2212,8 +2550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1F7A94-D1C6-4537-A70E-D5B7DD1165E4}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4079,19 +4417,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D010D53-A2B8-4D7D-8239-2883E618B035}">
   <dimension ref="A1:DD16"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="CU1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DC1" sqref="DC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.6640625" customWidth="1"/>
     <col min="2" max="2" width="116.109375" customWidth="1"/>
-    <col min="3" max="65" width="30" customWidth="1"/>
-    <col min="67" max="96" width="30" customWidth="1"/>
-    <col min="97" max="97" width="43" customWidth="1"/>
-    <col min="98" max="100" width="30" customWidth="1"/>
+    <col min="3" max="28" width="30" customWidth="1"/>
+    <col min="30" max="92" width="30" customWidth="1"/>
+    <col min="93" max="93" width="43" customWidth="1"/>
+    <col min="94" max="99" width="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:108" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4101,122 +4439,122 @@
       <c r="B1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="16"/>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="16"/>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="16"/>
-      <c r="AT1" s="16"/>
-      <c r="AU1" s="16"/>
-      <c r="AV1" s="16"/>
-      <c r="AW1" s="16"/>
-      <c r="AX1" s="16"/>
-      <c r="AY1" s="16"/>
-      <c r="AZ1" s="16"/>
-      <c r="BA1" s="16"/>
-      <c r="BB1" s="16"/>
-      <c r="BC1" s="16"/>
-      <c r="BD1" s="16"/>
-      <c r="BE1" s="16"/>
-      <c r="BF1" s="16"/>
-      <c r="BG1" s="16"/>
-      <c r="BH1" s="16"/>
-      <c r="BI1" s="16"/>
-      <c r="BJ1" s="16"/>
-      <c r="BK1" s="16"/>
-      <c r="BL1" s="16"/>
-      <c r="BM1" s="16"/>
-      <c r="BN1" s="16"/>
-      <c r="BO1" s="16"/>
-      <c r="BP1" s="16"/>
-      <c r="BQ1" s="16"/>
-      <c r="BR1" s="16"/>
-      <c r="BS1" s="16"/>
-      <c r="BT1" s="16"/>
-      <c r="BU1" s="16"/>
-      <c r="BV1" s="16"/>
-      <c r="BW1" s="16"/>
-      <c r="BX1" s="16"/>
-      <c r="BY1" s="16"/>
-      <c r="BZ1" s="16"/>
-      <c r="CA1" s="16"/>
-      <c r="CB1" s="16"/>
-      <c r="CC1" s="16"/>
-      <c r="CD1" s="16"/>
-      <c r="CE1" s="16"/>
-      <c r="CF1" s="16"/>
-      <c r="CG1" s="16"/>
-      <c r="CH1" s="16"/>
-      <c r="CI1" s="16"/>
-      <c r="CJ1" s="16"/>
-      <c r="CK1" s="16" t="s">
+      <c r="C1" s="78"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81"/>
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="82"/>
+      <c r="AD1" s="82"/>
+      <c r="AE1" s="82"/>
+      <c r="AF1" s="82"/>
+      <c r="AG1" s="82"/>
+      <c r="AH1" s="83"/>
+      <c r="AI1" s="83"/>
+      <c r="AJ1" s="83"/>
+      <c r="AK1" s="83"/>
+      <c r="AL1" s="83"/>
+      <c r="AM1" s="83"/>
+      <c r="AN1" s="83"/>
+      <c r="AO1" s="84"/>
+      <c r="AP1" s="84"/>
+      <c r="AQ1" s="84"/>
+      <c r="AR1" s="84"/>
+      <c r="AS1" s="84"/>
+      <c r="AT1" s="84"/>
+      <c r="AU1" s="84"/>
+      <c r="AV1" s="84"/>
+      <c r="AW1" s="84"/>
+      <c r="AX1" s="85"/>
+      <c r="AY1" s="85"/>
+      <c r="AZ1" s="85"/>
+      <c r="BA1" s="85"/>
+      <c r="BB1" s="85"/>
+      <c r="BC1" s="86"/>
+      <c r="BD1" s="86"/>
+      <c r="BE1" s="86"/>
+      <c r="BF1" s="86"/>
+      <c r="BG1" s="87"/>
+      <c r="BH1" s="87"/>
+      <c r="BI1" s="87"/>
+      <c r="BJ1" s="88"/>
+      <c r="BK1" s="88"/>
+      <c r="BL1" s="89"/>
+      <c r="BM1" s="89"/>
+      <c r="BN1" s="89"/>
+      <c r="BO1" s="90"/>
+      <c r="BP1" s="90"/>
+      <c r="BQ1" s="90"/>
+      <c r="BR1" s="91"/>
+      <c r="BS1" s="91"/>
+      <c r="BT1" s="91"/>
+      <c r="BU1" s="91"/>
+      <c r="BV1" s="91"/>
+      <c r="BW1" s="91"/>
+      <c r="BX1" s="91"/>
+      <c r="BY1" s="91"/>
+      <c r="BZ1" s="91"/>
+      <c r="CA1" s="91"/>
+      <c r="CB1" s="91"/>
+      <c r="CC1" s="91"/>
+      <c r="CD1" s="91"/>
+      <c r="CE1" s="91"/>
+      <c r="CF1" s="91"/>
+      <c r="CG1" s="91"/>
+      <c r="CH1" s="92"/>
+      <c r="CI1" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="CL1" s="16" t="s">
+      <c r="CJ1" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="CM1" s="16" t="s">
+      <c r="CK1" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="CN1" s="16" t="s">
+      <c r="CL1" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="CO1" s="16" t="s">
+      <c r="CM1" s="93"/>
+      <c r="CN1" s="93"/>
+      <c r="CO1" s="93"/>
+      <c r="CP1" s="93"/>
+      <c r="CQ1" s="94"/>
+      <c r="CR1" s="94"/>
+      <c r="CS1" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="CP1" s="16"/>
-      <c r="CQ1" s="16"/>
-      <c r="CR1" s="16"/>
-      <c r="CS1" s="16"/>
-      <c r="CT1" s="16"/>
-      <c r="CU1" s="16"/>
-      <c r="CV1" s="17"/>
-      <c r="CW1" s="17"/>
-      <c r="CX1" s="17"/>
-      <c r="CY1" s="16"/>
-      <c r="CZ1" s="16"/>
-      <c r="DA1" s="16"/>
-      <c r="DB1" s="16"/>
-      <c r="DC1" s="16"/>
-      <c r="DD1" s="16"/>
+      <c r="CT1" s="95"/>
+      <c r="CU1" s="95"/>
+      <c r="CV1" s="96"/>
+      <c r="CW1" s="96"/>
+      <c r="CX1" s="96"/>
+      <c r="CY1" s="95"/>
+      <c r="CZ1" s="95"/>
+      <c r="DA1" s="95"/>
+      <c r="DB1" s="95"/>
+      <c r="DC1" s="97"/>
+      <c r="DD1" s="3"/>
     </row>
     <row r="2" spans="1:108" s="3" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
@@ -4225,320 +4563,319 @@
       <c r="B2" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="R2" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="17" t="s">
+      <c r="S2" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="T2" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="U2" s="17" t="s">
+      <c r="U2" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="V2" s="17" t="s">
+      <c r="V2" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="W2" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="X2" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y2" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z2" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA2" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB2" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC2" s="50" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD2" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="AE2" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF2" s="50" t="s">
+        <v>286</v>
+      </c>
+      <c r="AG2" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="AH2" s="52" t="s">
+        <v>221</v>
+      </c>
+      <c r="AI2" s="52" t="s">
+        <v>223</v>
+      </c>
+      <c r="AJ2" s="52" t="s">
+        <v>225</v>
+      </c>
+      <c r="AK2" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="AL2" s="52" t="s">
+        <v>229</v>
+      </c>
+      <c r="AM2" s="52" t="s">
+        <v>217</v>
+      </c>
+      <c r="AN2" s="52" t="s">
+        <v>219</v>
+      </c>
+      <c r="AO2" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="AP2" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="AQ2" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="AR2" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="AS2" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="AT2" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="AU2" s="54" t="s">
+        <v>173</v>
+      </c>
+      <c r="AV2" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW2" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="AX2" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="W2" s="17" t="s">
+      <c r="AY2" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="X2" s="17" t="s">
+      <c r="AZ2" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="BA2" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="Z2" s="17" t="s">
+      <c r="BB2" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="AA2" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB2" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC2" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="AD2" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="AE2" s="17" t="s">
+      <c r="BC2" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="BD2" s="58" t="s">
+        <v>144</v>
+      </c>
+      <c r="BE2" s="58" t="s">
+        <v>145</v>
+      </c>
+      <c r="BF2" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="BG2" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="BH2" s="60" t="s">
+        <v>200</v>
+      </c>
+      <c r="BI2" s="60" t="s">
+        <v>206</v>
+      </c>
+      <c r="BJ2" s="62" t="s">
+        <v>183</v>
+      </c>
+      <c r="BK2" s="62" t="s">
+        <v>185</v>
+      </c>
+      <c r="BL2" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="AF2" s="17" t="s">
+      <c r="BM2" s="64" t="s">
+        <v>212</v>
+      </c>
+      <c r="BN2" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="BO2" s="66" t="s">
+        <v>232</v>
+      </c>
+      <c r="BP2" s="66" t="s">
+        <v>235</v>
+      </c>
+      <c r="BQ2" s="66" t="s">
+        <v>238</v>
+      </c>
+      <c r="BR2" s="68" t="s">
+        <v>240</v>
+      </c>
+      <c r="BS2" s="68" t="s">
+        <v>108</v>
+      </c>
+      <c r="BT2" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="AG2" s="17" t="s">
+      <c r="BU2" s="68" t="s">
         <v>111</v>
       </c>
-      <c r="AH2" s="17" t="s">
+      <c r="BV2" s="68" t="s">
         <v>116</v>
       </c>
-      <c r="AI2" s="17" t="s">
+      <c r="BW2" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="AJ2" s="17" t="s">
+      <c r="BX2" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="AK2" s="17" t="s">
+      <c r="BY2" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="AL2" s="17" t="s">
+      <c r="BZ2" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="AM2" s="17" t="s">
+      <c r="CA2" s="68" t="s">
         <v>122</v>
       </c>
-      <c r="AN2" s="17" t="s">
+      <c r="CB2" s="68" t="s">
         <v>123</v>
       </c>
-      <c r="AO2" s="17" t="s">
+      <c r="CC2" s="68" t="s">
         <v>124</v>
       </c>
-      <c r="AP2" s="17" t="s">
+      <c r="CD2" s="68" t="s">
         <v>124</v>
       </c>
-      <c r="AQ2" s="17" t="s">
+      <c r="CE2" s="68" t="s">
         <v>129</v>
       </c>
-      <c r="AR2" s="17" t="s">
+      <c r="CF2" s="68" t="s">
         <v>130</v>
       </c>
-      <c r="AS2" s="17" t="s">
+      <c r="CG2" s="68" t="s">
         <v>132</v>
       </c>
-      <c r="AT2" s="17" t="s">
+      <c r="CH2" s="70" t="s">
+        <v>242</v>
+      </c>
+      <c r="CI2" s="70" t="s">
+        <v>246</v>
+      </c>
+      <c r="CJ2" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="CK2" s="70" t="s">
+        <v>250</v>
+      </c>
+      <c r="CL2" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="CM2" s="72" t="s">
+        <v>255</v>
+      </c>
+      <c r="CN2" s="72" t="s">
+        <v>261</v>
+      </c>
+      <c r="CO2" s="72" t="s">
+        <v>262</v>
+      </c>
+      <c r="CP2" s="72" t="s">
+        <v>264</v>
+      </c>
+      <c r="CQ2" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="AU2" s="17" t="s">
+      <c r="CR2" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="AV2" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="AW2" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="AX2" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="AY2" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="AZ2" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="BA2" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="BB2" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="BC2" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="BD2" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="BE2" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="BF2" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="BG2" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="BH2" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="BI2" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="BJ2" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="BK2" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="BL2" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="BM2" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="BN2" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="BO2" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="BP2" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="BQ2" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="BR2" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="BS2" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="BT2" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="BU2" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="BV2" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="BW2" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="BX2" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="BY2" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="BZ2" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="CA2" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="CB2" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="CC2" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="CD2" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="CE2" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="CF2" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="CG2" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="CH2" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="CI2" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="CJ2" s="17"/>
-      <c r="CK2" s="17" t="s">
-        <v>242</v>
-      </c>
-      <c r="CL2" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="CM2" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="CN2" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="CO2" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="CP2" s="17" t="s">
+      <c r="CS2" s="74" t="s">
         <v>252</v>
       </c>
-      <c r="CQ2" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="CR2" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="CS2" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="CT2" s="17" t="s">
-        <v>264</v>
-      </c>
-      <c r="CU2" s="17" t="s">
+      <c r="CT2" s="76" t="s">
         <v>267</v>
       </c>
-      <c r="CV2" s="17" t="s">
+      <c r="CU2" s="76" t="s">
         <v>269</v>
       </c>
-      <c r="CW2" s="17" t="s">
+      <c r="CV2" s="76" t="s">
         <v>272</v>
       </c>
-      <c r="CX2" s="17" t="s">
+      <c r="CW2" s="76" t="s">
         <v>275</v>
       </c>
-      <c r="CY2" s="17" t="s">
+      <c r="CX2" s="76" t="s">
         <v>276</v>
       </c>
-      <c r="CZ2" s="17" t="s">
+      <c r="CY2" s="76" t="s">
         <v>277</v>
       </c>
-      <c r="DA2" s="17" t="s">
+      <c r="CZ2" s="76" t="s">
         <v>280</v>
       </c>
-      <c r="DB2" s="17" t="s">
+      <c r="DA2" s="76" t="s">
         <v>281</v>
       </c>
-      <c r="DC2" s="17" t="s">
+      <c r="DB2" s="76" t="s">
         <v>285</v>
       </c>
-      <c r="DD2" s="17"/>
+      <c r="DC2" s="99"/>
     </row>
     <row r="3" spans="1:108" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
@@ -4547,312 +4884,311 @@
       <c r="B3" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17" t="s">
+      <c r="C3" s="98"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="R3" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="S3" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="T3" s="17" t="s">
+      <c r="T3" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="U3" s="17" t="s">
+      <c r="U3" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="V3" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="W3" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="X3" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA3" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB3" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC3" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="W3" s="17" t="s">
+      <c r="AD3" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE3" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF3" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG3" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH3" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI3" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ3" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK3" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL3" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM3" s="52"/>
+      <c r="AN3" s="52"/>
+      <c r="AO3" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP3" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ3" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR3" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS3" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="X3" s="17" t="s">
+      <c r="AT3" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU3" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="AV3" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="Y3" s="17" t="s">
+      <c r="AW3" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX3" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="AY3" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="AZ3" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="BA3" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="Z3" s="17" t="s">
+      <c r="BB3" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="AA3" s="17" t="s">
+      <c r="BC3" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="AB3" s="17" t="s">
+      <c r="BD3" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="AC3" s="17" t="s">
+      <c r="BE3" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="BF3" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="BG3" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="BH3" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI3" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="BJ3" s="62" t="s">
+        <v>186</v>
+      </c>
+      <c r="BK3" s="62" t="s">
+        <v>186</v>
+      </c>
+      <c r="BL3" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="BM3" s="64" t="s">
+        <v>211</v>
+      </c>
+      <c r="BN3" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="BO3" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="BP3" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="BQ3" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="BR3" s="68" t="s">
+        <v>211</v>
+      </c>
+      <c r="BS3" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="BT3" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="BU3" s="68" t="s">
+        <v>92</v>
+      </c>
+      <c r="BV3" s="68" t="s">
+        <v>117</v>
+      </c>
+      <c r="BW3" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="BX3" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="BY3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AD3" s="17" t="s">
+      <c r="BZ3" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="CA3" s="68" t="s">
+        <v>128</v>
+      </c>
+      <c r="CB3" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="CC3" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="CD3" s="68" t="s">
+        <v>125</v>
+      </c>
+      <c r="CE3" s="68" t="s">
+        <v>92</v>
+      </c>
+      <c r="CF3" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="CG3" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="CH3" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="CI3" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="CJ3" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="CK3" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="CL3" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="CM3" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="CN3" s="72" t="s">
+        <v>259</v>
+      </c>
+      <c r="CO3" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP3" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="AE3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF3" s="17" t="s">
+      <c r="CQ3" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="CR3" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="CS3" s="74" t="s">
+        <v>186</v>
+      </c>
+      <c r="CT3" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="CU3" s="76" t="s">
+        <v>270</v>
+      </c>
+      <c r="CV3" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="CW3" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="CX3" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="CY3" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="CZ3" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="DA3" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="DB3" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="AG3" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="AH3" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="AK3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="AL3" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM3" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="AN3" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO3" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP3" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="AQ3" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="AR3" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="AS3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="AT3" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AU3" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="AW3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="AX3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="AY3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="AZ3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="BA3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="BB3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="BC3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="BD3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="BE3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="BF3" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="BG3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="BH3" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="BI3" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="BJ3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="BK3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="BL3" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="BM3" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="BN3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="BO3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="BP3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="BQ3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="BR3" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="BS3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="BT3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="BU3" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="BV3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="BW3" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="BX3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="BY3" s="17"/>
-      <c r="BZ3" s="17"/>
-      <c r="CA3" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="CB3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="CC3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="CD3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="CE3" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="CF3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="CG3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="CH3" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="CI3" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="CJ3" s="17"/>
-      <c r="CK3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="CL3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="CM3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="CN3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="CO3" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="CP3" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="CQ3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="CR3" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="CS3" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="CT3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="CU3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="CV3" s="17" t="s">
-        <v>270</v>
-      </c>
-      <c r="CW3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="CX3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="CY3" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="CZ3" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="DA3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="DB3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="DC3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="DD3" s="17"/>
+      <c r="DC3" s="99"/>
     </row>
     <row r="4" spans="1:108" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="s">
@@ -4861,190 +5197,189 @@
       <c r="B4" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17" t="s">
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17" t="s">
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1" t="s">
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="W4" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="X4" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y4" s="46"/>
+      <c r="Z4" s="49"/>
+      <c r="AA4" s="49"/>
+      <c r="AB4" s="49"/>
+      <c r="AC4" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="AD4" s="51"/>
+      <c r="AE4" s="50"/>
+      <c r="AF4" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG4" s="51"/>
+      <c r="AH4" s="53"/>
+      <c r="AI4" s="53"/>
+      <c r="AJ4" s="52"/>
+      <c r="AK4" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL4" s="53"/>
+      <c r="AM4" s="53"/>
+      <c r="AN4" s="53"/>
+      <c r="AO4" s="55"/>
+      <c r="AP4" s="55"/>
+      <c r="AQ4" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR4" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="AS4" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="AT4" s="55"/>
+      <c r="AU4" s="55"/>
+      <c r="AV4" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="AW4" s="55" t="s">
+        <v>180</v>
+      </c>
+      <c r="AX4" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="AY4" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="AZ4" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AC4" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD4" s="17"/>
-      <c r="AE4" s="17" t="s">
+      <c r="BA4" s="57"/>
+      <c r="BB4" s="57"/>
+      <c r="BC4" s="59" t="s">
+        <v>140</v>
+      </c>
+      <c r="BD4" s="59" t="s">
+        <v>142</v>
+      </c>
+      <c r="BE4" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="BF4" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="BG4" s="61" t="s">
+        <v>204</v>
+      </c>
+      <c r="BH4" s="61" t="s">
+        <v>201</v>
+      </c>
+      <c r="BI4" s="61"/>
+      <c r="BJ4" s="63"/>
+      <c r="BK4" s="63"/>
+      <c r="BL4" s="65" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM4" s="65"/>
+      <c r="BN4" s="65" t="s">
+        <v>215</v>
+      </c>
+      <c r="BO4" s="67" t="s">
+        <v>233</v>
+      </c>
+      <c r="BP4" s="67" t="s">
+        <v>236</v>
+      </c>
+      <c r="BQ4" s="67"/>
+      <c r="BR4" s="69"/>
+      <c r="BS4" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="AF4" s="17" t="s">
+      <c r="BT4" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="AG4" s="17"/>
-      <c r="AH4" s="17"/>
-      <c r="AI4" s="17"/>
-      <c r="AJ4" s="17"/>
-      <c r="AK4" s="17"/>
-      <c r="AL4" s="17"/>
-      <c r="AM4" s="17"/>
-      <c r="AN4" s="17"/>
-      <c r="AO4" s="17"/>
-      <c r="AP4" s="17"/>
-      <c r="AQ4" s="1"/>
-      <c r="AR4" s="1"/>
-      <c r="AS4" s="1"/>
-      <c r="AT4" s="1"/>
-      <c r="AU4" s="1"/>
-      <c r="AV4" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="AW4" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AX4" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AY4" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AZ4" s="1"/>
-      <c r="BA4" s="1"/>
-      <c r="BB4" s="1"/>
-      <c r="BC4" s="1"/>
-      <c r="BD4" s="1"/>
-      <c r="BE4" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="BF4" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="BG4" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="BH4" s="1"/>
-      <c r="BI4" s="1"/>
-      <c r="BJ4" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="BK4" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="BL4" s="1"/>
-      <c r="BM4" s="1"/>
-      <c r="BN4" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="BO4" s="1"/>
-      <c r="BP4" s="17"/>
-      <c r="BQ4" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="BR4" s="1"/>
-      <c r="BS4" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="BT4" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="BU4" s="1"/>
-      <c r="BV4" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="BW4" s="1"/>
-      <c r="BX4" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="BY4" s="1"/>
-      <c r="BZ4" s="1"/>
-      <c r="CA4" s="1"/>
-      <c r="CB4" s="1"/>
-      <c r="CC4" s="17"/>
-      <c r="CD4" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="CE4" s="1"/>
-      <c r="CF4" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="CG4" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="CH4" s="1"/>
-      <c r="CI4" s="1"/>
-      <c r="CJ4" s="1"/>
-      <c r="CK4" s="1" t="s">
+      <c r="BU4" s="68"/>
+      <c r="BV4" s="68"/>
+      <c r="BW4" s="68"/>
+      <c r="BX4" s="68"/>
+      <c r="BY4" s="68"/>
+      <c r="BZ4" s="68"/>
+      <c r="CA4" s="68"/>
+      <c r="CB4" s="68"/>
+      <c r="CC4" s="68"/>
+      <c r="CD4" s="68"/>
+      <c r="CE4" s="69"/>
+      <c r="CF4" s="69"/>
+      <c r="CG4" s="69"/>
+      <c r="CH4" s="71" t="s">
         <v>243</v>
       </c>
-      <c r="CL4" s="1" t="s">
+      <c r="CI4" s="71" t="s">
         <v>245</v>
       </c>
-      <c r="CM4" s="1" t="s">
+      <c r="CJ4" s="71" t="s">
         <v>247</v>
       </c>
-      <c r="CN4" s="1"/>
-      <c r="CO4" s="1"/>
-      <c r="CP4" s="1"/>
-      <c r="CQ4" s="1" t="s">
+      <c r="CK4" s="71"/>
+      <c r="CL4" s="71"/>
+      <c r="CM4" s="73" t="s">
         <v>256</v>
       </c>
-      <c r="CR4" s="1" t="s">
+      <c r="CN4" s="73" t="s">
         <v>260</v>
       </c>
-      <c r="CS4" s="17"/>
-      <c r="CT4" s="17"/>
-      <c r="CU4" s="1"/>
-      <c r="CV4" s="1"/>
-      <c r="CW4" s="1"/>
-      <c r="CX4" s="1"/>
-      <c r="CY4" s="1"/>
-      <c r="CZ4" s="1"/>
-      <c r="DA4" s="1"/>
-      <c r="DB4" s="1"/>
-      <c r="DC4" s="1" t="s">
+      <c r="CO4" s="72"/>
+      <c r="CP4" s="72"/>
+      <c r="CQ4" s="75"/>
+      <c r="CR4" s="75"/>
+      <c r="CS4" s="75"/>
+      <c r="CT4" s="77"/>
+      <c r="CU4" s="77"/>
+      <c r="CV4" s="77"/>
+      <c r="CW4" s="77"/>
+      <c r="CX4" s="77"/>
+      <c r="CY4" s="77"/>
+      <c r="CZ4" s="77"/>
+      <c r="DA4" s="77"/>
+      <c r="DB4" s="77" t="s">
         <v>284</v>
       </c>
-      <c r="DD4" s="1"/>
+      <c r="DC4" s="99"/>
     </row>
     <row r="5" spans="1:108" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
@@ -5053,312 +5388,311 @@
       <c r="B5" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="N5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="O5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="P5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="Q5" s="17" t="s">
+      <c r="Q5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="R5" s="17" t="s">
+      <c r="R5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="S5" s="17" t="s">
+      <c r="S5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="T5" s="17" t="s">
+      <c r="T5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17" t="s">
+      <c r="U5" s="44"/>
+      <c r="V5" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="W5" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="X5" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y5" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z5" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA5" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB5" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC5" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="AD5" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="AE5" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="AF5" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="AG5" s="50"/>
+      <c r="AH5" s="52" t="s">
+        <v>216</v>
+      </c>
+      <c r="AI5" s="52" t="s">
+        <v>216</v>
+      </c>
+      <c r="AJ5" s="52" t="s">
+        <v>216</v>
+      </c>
+      <c r="AK5" s="52" t="s">
+        <v>216</v>
+      </c>
+      <c r="AL5" s="52" t="s">
+        <v>216</v>
+      </c>
+      <c r="AM5" s="52" t="s">
+        <v>216</v>
+      </c>
+      <c r="AN5" s="52" t="s">
+        <v>216</v>
+      </c>
+      <c r="AO5" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="AP5" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="AQ5" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="AR5" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="AS5" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="AT5" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="AU5" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="AV5" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="AW5" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="AX5" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="W5" s="17" t="s">
+      <c r="AY5" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="X5" s="17" t="s">
+      <c r="AZ5" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="Y5" s="17" t="s">
+      <c r="BA5" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="Z5" s="17" t="s">
+      <c r="BB5" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="AA5" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB5" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC5" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="AD5" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE5" s="17" t="s">
+      <c r="BC5" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="BD5" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="BE5" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="BF5" s="58"/>
+      <c r="BG5" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="BH5" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="BI5" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="BJ5" s="62" t="s">
+        <v>182</v>
+      </c>
+      <c r="BK5" s="62" t="s">
+        <v>182</v>
+      </c>
+      <c r="BL5" s="64" t="s">
+        <v>208</v>
+      </c>
+      <c r="BM5" s="64" t="s">
+        <v>208</v>
+      </c>
+      <c r="BN5" s="64" t="s">
+        <v>208</v>
+      </c>
+      <c r="BO5" s="66" t="s">
+        <v>231</v>
+      </c>
+      <c r="BP5" s="66" t="s">
+        <v>231</v>
+      </c>
+      <c r="BQ5" s="66" t="s">
+        <v>231</v>
+      </c>
+      <c r="BR5" s="68" t="s">
+        <v>231</v>
+      </c>
+      <c r="BS5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AF5" s="17" t="s">
+      <c r="BT5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AG5" s="17" t="s">
+      <c r="BU5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AH5" s="17" t="s">
+      <c r="BV5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AI5" s="17" t="s">
+      <c r="BW5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AJ5" s="17" t="s">
+      <c r="BX5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AK5" s="17" t="s">
+      <c r="BY5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AL5" s="17" t="s">
+      <c r="BZ5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AM5" s="17" t="s">
+      <c r="CA5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AN5" s="17" t="s">
+      <c r="CB5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AO5" s="17" t="s">
+      <c r="CC5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AP5" s="17" t="s">
+      <c r="CD5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AQ5" s="17" t="s">
+      <c r="CE5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AR5" s="17" t="s">
+      <c r="CF5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AS5" s="17" t="s">
+      <c r="CG5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AT5" s="17" t="s">
+      <c r="CH5" s="70" t="s">
+        <v>137</v>
+      </c>
+      <c r="CI5" s="70" t="s">
+        <v>137</v>
+      </c>
+      <c r="CJ5" s="70" t="s">
+        <v>137</v>
+      </c>
+      <c r="CK5" s="70" t="s">
+        <v>137</v>
+      </c>
+      <c r="CL5" s="70"/>
+      <c r="CM5" s="72" t="s">
+        <v>254</v>
+      </c>
+      <c r="CN5" s="72" t="s">
+        <v>254</v>
+      </c>
+      <c r="CO5" s="72" t="s">
+        <v>254</v>
+      </c>
+      <c r="CP5" s="72" t="s">
+        <v>254</v>
+      </c>
+      <c r="CQ5" s="75" t="s">
         <v>134</v>
       </c>
-      <c r="AU5" s="17" t="s">
+      <c r="CR5" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="AV5" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="AW5" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="AX5" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="AY5" s="17"/>
-      <c r="AZ5" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="BA5" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="BB5" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="BC5" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="BD5" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="BE5" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="BF5" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="BG5" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="BH5" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="BI5" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="BJ5" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="BK5" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="BL5" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="BM5" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="BN5" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="BO5" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="BP5" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="BQ5" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="BR5" s="17"/>
-      <c r="BS5" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="BT5" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="BU5" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="BV5" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="BW5" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="BX5" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="BY5" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="BZ5" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="CA5" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="CB5" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="CC5" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="CD5" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="CE5" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="CF5" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="CG5" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="CH5" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="CI5" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="CJ5" s="17"/>
-      <c r="CK5" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="CL5" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="CM5" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="CN5" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="CO5" s="17"/>
-      <c r="CP5" s="17" t="s">
+      <c r="CS5" s="74" t="s">
         <v>251</v>
       </c>
-      <c r="CQ5" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="CR5" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="CS5" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="CT5" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="CU5" s="17" t="s">
+      <c r="CT5" s="76" t="s">
         <v>266</v>
       </c>
-      <c r="CV5" s="17" t="s">
+      <c r="CU5" s="76" t="s">
         <v>266</v>
       </c>
-      <c r="CW5" s="17" t="s">
+      <c r="CV5" s="76" t="s">
         <v>266</v>
       </c>
-      <c r="CX5" s="17" t="s">
+      <c r="CW5" s="76" t="s">
         <v>266</v>
       </c>
-      <c r="CY5" s="17" t="s">
+      <c r="CX5" s="76" t="s">
         <v>266</v>
       </c>
-      <c r="CZ5" s="17" t="s">
+      <c r="CY5" s="76" t="s">
         <v>266</v>
       </c>
-      <c r="DA5" s="17" t="s">
+      <c r="CZ5" s="76" t="s">
         <v>266</v>
       </c>
-      <c r="DB5" s="17" t="s">
+      <c r="DA5" s="76" t="s">
         <v>266</v>
       </c>
-      <c r="DC5" s="17" t="s">
+      <c r="DB5" s="76" t="s">
         <v>266</v>
       </c>
-      <c r="DD5" s="17"/>
+      <c r="DC5" s="99"/>
     </row>
     <row r="6" spans="1:108" s="3" customFormat="1" ht="52.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="42" t="s">
@@ -5367,316 +5701,315 @@
       <c r="B6" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="101" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="101" t="s">
         <v>69</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="101" t="s">
         <v>70</v>
       </c>
-      <c r="R6" s="18" t="s">
+      <c r="R6" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="S6" s="18" t="s">
+      <c r="S6" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="T6" s="18" t="s">
+      <c r="T6" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18" t="s">
+      <c r="U6" s="101"/>
+      <c r="V6" s="101" t="s">
+        <v>99</v>
+      </c>
+      <c r="W6" s="101" t="s">
+        <v>100</v>
+      </c>
+      <c r="X6" s="101" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y6" s="101" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z6" s="101" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA6" s="101" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB6" s="101" t="s">
+        <v>156</v>
+      </c>
+      <c r="AC6" s="101" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD6" s="101" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE6" s="101" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF6" s="101" t="s">
+        <v>195</v>
+      </c>
+      <c r="AG6" s="101" t="s">
+        <v>198</v>
+      </c>
+      <c r="AH6" s="101" t="s">
+        <v>222</v>
+      </c>
+      <c r="AI6" s="101" t="s">
+        <v>224</v>
+      </c>
+      <c r="AJ6" s="101" t="s">
+        <v>227</v>
+      </c>
+      <c r="AK6" s="101" t="s">
+        <v>228</v>
+      </c>
+      <c r="AL6" s="101" t="s">
+        <v>230</v>
+      </c>
+      <c r="AM6" s="101" t="s">
+        <v>218</v>
+      </c>
+      <c r="AN6" s="101" t="s">
+        <v>220</v>
+      </c>
+      <c r="AO6" s="101" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP6" s="101" t="s">
+        <v>162</v>
+      </c>
+      <c r="AQ6" s="101" t="s">
+        <v>167</v>
+      </c>
+      <c r="AR6" s="101" t="s">
+        <v>168</v>
+      </c>
+      <c r="AS6" s="101" t="s">
+        <v>171</v>
+      </c>
+      <c r="AT6" s="101" t="s">
+        <v>174</v>
+      </c>
+      <c r="AU6" s="101" t="s">
+        <v>175</v>
+      </c>
+      <c r="AV6" s="101" t="s">
+        <v>178</v>
+      </c>
+      <c r="AW6" s="101" t="s">
+        <v>181</v>
+      </c>
+      <c r="AX6" s="101" t="s">
         <v>83</v>
       </c>
-      <c r="W6" s="18" t="s">
+      <c r="AY6" s="101" t="s">
         <v>85</v>
       </c>
-      <c r="X6" s="18" t="s">
+      <c r="AZ6" s="101" t="s">
         <v>89</v>
       </c>
-      <c r="Y6" s="18" t="s">
+      <c r="BA6" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="Z6" s="18" t="s">
+      <c r="BB6" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="AA6" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB6" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="AC6" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="AD6" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE6" s="18" t="s">
+      <c r="BC6" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="BD6" s="101" t="s">
+        <v>143</v>
+      </c>
+      <c r="BE6" s="101" t="s">
+        <v>147</v>
+      </c>
+      <c r="BF6" s="101" t="s">
+        <v>150</v>
+      </c>
+      <c r="BG6" s="101" t="s">
+        <v>205</v>
+      </c>
+      <c r="BH6" s="101" t="s">
+        <v>202</v>
+      </c>
+      <c r="BI6" s="101" t="s">
+        <v>207</v>
+      </c>
+      <c r="BJ6" s="101" t="s">
+        <v>184</v>
+      </c>
+      <c r="BK6" s="101" t="s">
+        <v>187</v>
+      </c>
+      <c r="BL6" s="101" t="s">
+        <v>210</v>
+      </c>
+      <c r="BM6" s="101" t="s">
+        <v>213</v>
+      </c>
+      <c r="BN6" s="101" t="s">
+        <v>214</v>
+      </c>
+      <c r="BO6" s="101" t="s">
+        <v>234</v>
+      </c>
+      <c r="BP6" s="101" t="s">
+        <v>237</v>
+      </c>
+      <c r="BQ6" s="101" t="s">
+        <v>239</v>
+      </c>
+      <c r="BR6" s="101" t="s">
+        <v>241</v>
+      </c>
+      <c r="BS6" s="101" t="s">
         <v>109</v>
       </c>
-      <c r="AF6" s="18" t="s">
+      <c r="BT6" s="101" t="s">
         <v>115</v>
       </c>
-      <c r="AG6" s="18" t="s">
+      <c r="BU6" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="AH6" s="18" t="s">
+      <c r="BV6" s="101" t="s">
         <v>118</v>
       </c>
-      <c r="AI6" s="18" t="s">
+      <c r="BW6" s="101" t="s">
         <v>118</v>
       </c>
-      <c r="AJ6" s="18" t="s">
+      <c r="BX6" s="101" t="s">
         <v>118</v>
       </c>
-      <c r="AK6" s="18" t="s">
+      <c r="BY6" s="101" t="s">
         <v>118</v>
       </c>
-      <c r="AL6" s="18" t="s">
+      <c r="BZ6" s="101" t="s">
         <v>118</v>
       </c>
-      <c r="AM6" s="18" t="s">
+      <c r="CA6" s="101" t="s">
         <v>118</v>
       </c>
-      <c r="AN6" s="18" t="s">
+      <c r="CB6" s="101" t="s">
         <v>118</v>
       </c>
-      <c r="AO6" s="18" t="s">
+      <c r="CC6" s="101" t="s">
         <v>118</v>
       </c>
-      <c r="AP6" s="18" t="s">
+      <c r="CD6" s="101" t="s">
         <v>118</v>
       </c>
-      <c r="AQ6" s="18" t="s">
+      <c r="CE6" s="101" t="s">
         <v>118</v>
       </c>
-      <c r="AR6" s="18" t="s">
+      <c r="CF6" s="101" t="s">
         <v>118</v>
       </c>
-      <c r="AS6" s="18" t="s">
+      <c r="CG6" s="101" t="s">
         <v>133</v>
       </c>
-      <c r="AT6" s="18" t="s">
+      <c r="CH6" s="101" t="s">
+        <v>244</v>
+      </c>
+      <c r="CI6" s="101" t="s">
+        <v>248</v>
+      </c>
+      <c r="CJ6" s="101" t="s">
+        <v>42</v>
+      </c>
+      <c r="CK6" s="101" t="s">
+        <v>249</v>
+      </c>
+      <c r="CL6" s="101" t="s">
+        <v>45</v>
+      </c>
+      <c r="CM6" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="CN6" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="CO6" s="101" t="s">
+        <v>263</v>
+      </c>
+      <c r="CP6" s="101" t="s">
+        <v>265</v>
+      </c>
+      <c r="CQ6" s="101" t="s">
         <v>135</v>
       </c>
-      <c r="AU6" s="18" t="s">
+      <c r="CR6" s="101" t="s">
         <v>136</v>
       </c>
-      <c r="AV6" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW6" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="AX6" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="AY6" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="AZ6" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="BA6" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="BB6" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="BC6" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="BD6" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="BE6" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="BF6" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="BG6" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="BH6" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="BI6" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="BJ6" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="BK6" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="BL6" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="BM6" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="BN6" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="BO6" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="BP6" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="BQ6" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="BR6" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="BS6" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="BT6" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="BU6" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="BV6" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="BW6" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="BX6" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="BY6" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="BZ6" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="CA6" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="CB6" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="CC6" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="CD6" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="CE6" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="CF6" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="CG6" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="CH6" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="CI6" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="CJ6" s="18"/>
-      <c r="CK6" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="CL6" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="CM6" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="CN6" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="CO6" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="CP6" s="18" t="s">
+      <c r="CS6" s="101" t="s">
         <v>253</v>
       </c>
-      <c r="CQ6" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="CR6" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="CS6" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="CT6" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="CU6" s="18" t="s">
+      <c r="CT6" s="101" t="s">
         <v>268</v>
       </c>
-      <c r="CV6" s="18" t="s">
+      <c r="CU6" s="101" t="s">
         <v>271</v>
       </c>
-      <c r="CW6" s="18" t="s">
+      <c r="CV6" s="101" t="s">
         <v>273</v>
       </c>
-      <c r="CX6" s="18" t="s">
+      <c r="CW6" s="101" t="s">
         <v>274</v>
       </c>
-      <c r="CY6" s="18" t="s">
+      <c r="CX6" s="101" t="s">
         <v>278</v>
       </c>
-      <c r="CZ6" s="18" t="s">
+      <c r="CY6" s="101" t="s">
         <v>279</v>
       </c>
-      <c r="DA6" s="18" t="s">
+      <c r="CZ6" s="101" t="s">
         <v>283</v>
       </c>
-      <c r="DB6" s="18" t="s">
+      <c r="DA6" s="101" t="s">
         <v>282</v>
       </c>
-      <c r="DC6" s="19"/>
-      <c r="DD6" s="19"/>
+      <c r="DB6" s="102"/>
+      <c r="DC6" s="103"/>
     </row>
     <row r="7" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
@@ -5770,14 +6103,14 @@
       <c r="CK7" s="22"/>
       <c r="CL7" s="22"/>
       <c r="CM7" s="22"/>
-      <c r="CN7" s="22"/>
+      <c r="CN7" s="23"/>
       <c r="CO7" s="22"/>
       <c r="CP7" s="22"/>
       <c r="CQ7" s="22"/>
-      <c r="CR7" s="23"/>
+      <c r="CR7" s="22"/>
       <c r="CS7" s="22"/>
-      <c r="CT7" s="22"/>
-      <c r="CU7" s="23"/>
+      <c r="CT7" s="23"/>
+      <c r="CU7" s="22"/>
       <c r="CV7" s="22"/>
       <c r="CW7" s="22"/>
       <c r="CX7" s="22"/>
@@ -5785,8 +6118,7 @@
       <c r="CZ7" s="22"/>
       <c r="DA7" s="22"/>
       <c r="DB7" s="22"/>
-      <c r="DC7" s="22"/>
-      <c r="DD7" s="24"/>
+      <c r="DC7" s="24"/>
     </row>
     <row r="8" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
@@ -5874,20 +6206,20 @@
       <c r="CE8" s="12"/>
       <c r="CF8" s="12"/>
       <c r="CG8" s="12"/>
-      <c r="CH8" s="12"/>
-      <c r="CI8" s="12"/>
-      <c r="CJ8" s="12"/>
+      <c r="CH8" s="20"/>
+      <c r="CI8" s="20"/>
+      <c r="CJ8" s="20"/>
       <c r="CK8" s="20"/>
       <c r="CL8" s="20"/>
-      <c r="CM8" s="20"/>
-      <c r="CN8" s="20"/>
-      <c r="CO8" s="20"/>
-      <c r="CP8" s="20"/>
+      <c r="CM8" s="12"/>
+      <c r="CN8" s="13"/>
+      <c r="CO8" s="12"/>
+      <c r="CP8" s="12"/>
       <c r="CQ8" s="12"/>
-      <c r="CR8" s="13"/>
-      <c r="CS8" s="12"/>
-      <c r="CT8" s="12"/>
-      <c r="CU8" s="13"/>
+      <c r="CR8" s="12"/>
+      <c r="CS8" s="20"/>
+      <c r="CT8" s="13"/>
+      <c r="CU8" s="12"/>
       <c r="CV8" s="12"/>
       <c r="CW8" s="12"/>
       <c r="CX8" s="12"/>
@@ -5895,8 +6227,7 @@
       <c r="CZ8" s="12"/>
       <c r="DA8" s="12"/>
       <c r="DB8" s="12"/>
-      <c r="DC8" s="12"/>
-      <c r="DD8" s="26"/>
+      <c r="DC8" s="26"/>
     </row>
     <row r="9" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
@@ -5984,20 +6315,20 @@
       <c r="CE9" s="12"/>
       <c r="CF9" s="12"/>
       <c r="CG9" s="12"/>
-      <c r="CH9" s="12"/>
-      <c r="CI9" s="12"/>
-      <c r="CJ9" s="12"/>
+      <c r="CH9" s="20"/>
+      <c r="CI9" s="20"/>
+      <c r="CJ9" s="20"/>
       <c r="CK9" s="20"/>
       <c r="CL9" s="20"/>
-      <c r="CM9" s="20"/>
-      <c r="CN9" s="20"/>
-      <c r="CO9" s="20"/>
-      <c r="CP9" s="20"/>
+      <c r="CM9" s="12"/>
+      <c r="CN9" s="13"/>
+      <c r="CO9" s="12"/>
+      <c r="CP9" s="12"/>
       <c r="CQ9" s="12"/>
-      <c r="CR9" s="13"/>
-      <c r="CS9" s="12"/>
-      <c r="CT9" s="12"/>
-      <c r="CU9" s="13"/>
+      <c r="CR9" s="12"/>
+      <c r="CS9" s="20"/>
+      <c r="CT9" s="13"/>
+      <c r="CU9" s="12"/>
       <c r="CV9" s="12"/>
       <c r="CW9" s="12"/>
       <c r="CX9" s="12"/>
@@ -6005,8 +6336,7 @@
       <c r="CZ9" s="12"/>
       <c r="DA9" s="12"/>
       <c r="DB9" s="12"/>
-      <c r="DC9" s="12"/>
-      <c r="DD9" s="26"/>
+      <c r="DC9" s="26"/>
     </row>
     <row r="10" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
@@ -6094,20 +6424,20 @@
       <c r="CE10" s="12"/>
       <c r="CF10" s="12"/>
       <c r="CG10" s="12"/>
-      <c r="CH10" s="12"/>
-      <c r="CI10" s="12"/>
-      <c r="CJ10" s="12"/>
+      <c r="CH10" s="20"/>
+      <c r="CI10" s="20"/>
+      <c r="CJ10" s="20"/>
       <c r="CK10" s="20"/>
       <c r="CL10" s="20"/>
-      <c r="CM10" s="20"/>
-      <c r="CN10" s="20"/>
-      <c r="CO10" s="20"/>
-      <c r="CP10" s="20"/>
+      <c r="CM10" s="12"/>
+      <c r="CN10" s="13"/>
+      <c r="CO10" s="12"/>
+      <c r="CP10" s="12"/>
       <c r="CQ10" s="12"/>
-      <c r="CR10" s="13"/>
-      <c r="CS10" s="12"/>
-      <c r="CT10" s="12"/>
-      <c r="CU10" s="13"/>
+      <c r="CR10" s="12"/>
+      <c r="CS10" s="20"/>
+      <c r="CT10" s="13"/>
+      <c r="CU10" s="12"/>
       <c r="CV10" s="12"/>
       <c r="CW10" s="12"/>
       <c r="CX10" s="12"/>
@@ -6115,8 +6445,7 @@
       <c r="CZ10" s="12"/>
       <c r="DA10" s="12"/>
       <c r="DB10" s="12"/>
-      <c r="DC10" s="12"/>
-      <c r="DD10" s="26"/>
+      <c r="DC10" s="26"/>
     </row>
     <row r="11" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
@@ -6204,20 +6533,20 @@
       <c r="CE11" s="12"/>
       <c r="CF11" s="12"/>
       <c r="CG11" s="12"/>
-      <c r="CH11" s="12"/>
-      <c r="CI11" s="12"/>
-      <c r="CJ11" s="12"/>
+      <c r="CH11" s="20"/>
+      <c r="CI11" s="20"/>
+      <c r="CJ11" s="20"/>
       <c r="CK11" s="20"/>
       <c r="CL11" s="20"/>
-      <c r="CM11" s="20"/>
-      <c r="CN11" s="20"/>
-      <c r="CO11" s="20"/>
-      <c r="CP11" s="20"/>
+      <c r="CM11" s="12"/>
+      <c r="CN11" s="13"/>
+      <c r="CO11" s="12"/>
+      <c r="CP11" s="12"/>
       <c r="CQ11" s="12"/>
-      <c r="CR11" s="13"/>
-      <c r="CS11" s="12"/>
-      <c r="CT11" s="12"/>
-      <c r="CU11" s="13"/>
+      <c r="CR11" s="12"/>
+      <c r="CS11" s="20"/>
+      <c r="CT11" s="13"/>
+      <c r="CU11" s="12"/>
       <c r="CV11" s="12"/>
       <c r="CW11" s="12"/>
       <c r="CX11" s="12"/>
@@ -6225,8 +6554,7 @@
       <c r="CZ11" s="12"/>
       <c r="DA11" s="12"/>
       <c r="DB11" s="12"/>
-      <c r="DC11" s="12"/>
-      <c r="DD11" s="26"/>
+      <c r="DC11" s="26"/>
     </row>
     <row r="12" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
@@ -6314,20 +6642,20 @@
       <c r="CE12" s="12"/>
       <c r="CF12" s="12"/>
       <c r="CG12" s="12"/>
-      <c r="CH12" s="12"/>
-      <c r="CI12" s="12"/>
-      <c r="CJ12" s="12"/>
+      <c r="CH12" s="20"/>
+      <c r="CI12" s="20"/>
+      <c r="CJ12" s="20"/>
       <c r="CK12" s="20"/>
       <c r="CL12" s="20"/>
-      <c r="CM12" s="20"/>
-      <c r="CN12" s="20"/>
-      <c r="CO12" s="20"/>
-      <c r="CP12" s="20"/>
+      <c r="CM12" s="12"/>
+      <c r="CN12" s="13"/>
+      <c r="CO12" s="12"/>
+      <c r="CP12" s="12"/>
       <c r="CQ12" s="12"/>
-      <c r="CR12" s="13"/>
-      <c r="CS12" s="12"/>
-      <c r="CT12" s="12"/>
-      <c r="CU12" s="13"/>
+      <c r="CR12" s="12"/>
+      <c r="CS12" s="20"/>
+      <c r="CT12" s="13"/>
+      <c r="CU12" s="12"/>
       <c r="CV12" s="12"/>
       <c r="CW12" s="12"/>
       <c r="CX12" s="12"/>
@@ -6335,8 +6663,7 @@
       <c r="CZ12" s="12"/>
       <c r="DA12" s="12"/>
       <c r="DB12" s="12"/>
-      <c r="DC12" s="12"/>
-      <c r="DD12" s="26"/>
+      <c r="DC12" s="26"/>
     </row>
     <row r="13" spans="1:108" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
@@ -6424,20 +6751,20 @@
       <c r="CE13" s="12"/>
       <c r="CF13" s="12"/>
       <c r="CG13" s="12"/>
-      <c r="CH13" s="12"/>
-      <c r="CI13" s="12"/>
-      <c r="CJ13" s="12"/>
+      <c r="CH13" s="20"/>
+      <c r="CI13" s="20"/>
+      <c r="CJ13" s="20"/>
       <c r="CK13" s="20"/>
       <c r="CL13" s="20"/>
-      <c r="CM13" s="20"/>
-      <c r="CN13" s="20"/>
-      <c r="CO13" s="20"/>
-      <c r="CP13" s="20"/>
+      <c r="CM13" s="12"/>
+      <c r="CN13" s="13"/>
+      <c r="CO13" s="12"/>
+      <c r="CP13" s="12"/>
       <c r="CQ13" s="12"/>
-      <c r="CR13" s="13"/>
-      <c r="CS13" s="12"/>
-      <c r="CT13" s="12"/>
-      <c r="CU13" s="13"/>
+      <c r="CR13" s="12"/>
+      <c r="CS13" s="20"/>
+      <c r="CT13" s="13"/>
+      <c r="CU13" s="12"/>
       <c r="CV13" s="12"/>
       <c r="CW13" s="12"/>
       <c r="CX13" s="12"/>
@@ -6445,8 +6772,7 @@
       <c r="CZ13" s="12"/>
       <c r="DA13" s="12"/>
       <c r="DB13" s="12"/>
-      <c r="DC13" s="12"/>
-      <c r="DD13" s="26"/>
+      <c r="DC13" s="26"/>
     </row>
     <row r="14" spans="1:108" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
@@ -6534,20 +6860,20 @@
       <c r="CE14" s="12"/>
       <c r="CF14" s="12"/>
       <c r="CG14" s="12"/>
-      <c r="CH14" s="12"/>
-      <c r="CI14" s="12"/>
-      <c r="CJ14" s="12"/>
+      <c r="CH14" s="20"/>
+      <c r="CI14" s="20"/>
+      <c r="CJ14" s="20"/>
       <c r="CK14" s="20"/>
       <c r="CL14" s="20"/>
-      <c r="CM14" s="20"/>
-      <c r="CN14" s="20"/>
-      <c r="CO14" s="20"/>
-      <c r="CP14" s="20"/>
+      <c r="CM14" s="12"/>
+      <c r="CN14" s="13"/>
+      <c r="CO14" s="12"/>
+      <c r="CP14" s="12"/>
       <c r="CQ14" s="12"/>
-      <c r="CR14" s="13"/>
-      <c r="CS14" s="12"/>
-      <c r="CT14" s="12"/>
-      <c r="CU14" s="13"/>
+      <c r="CR14" s="12"/>
+      <c r="CS14" s="20"/>
+      <c r="CT14" s="13"/>
+      <c r="CU14" s="12"/>
       <c r="CV14" s="12"/>
       <c r="CW14" s="12"/>
       <c r="CX14" s="12"/>
@@ -6555,8 +6881,7 @@
       <c r="CZ14" s="12"/>
       <c r="DA14" s="12"/>
       <c r="DB14" s="12"/>
-      <c r="DC14" s="12"/>
-      <c r="DD14" s="26"/>
+      <c r="DC14" s="26"/>
     </row>
     <row r="15" spans="1:108" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
@@ -6644,20 +6969,20 @@
       <c r="CE15" s="12"/>
       <c r="CF15" s="12"/>
       <c r="CG15" s="12"/>
-      <c r="CH15" s="12"/>
-      <c r="CI15" s="12"/>
-      <c r="CJ15" s="12"/>
+      <c r="CH15" s="20"/>
+      <c r="CI15" s="20"/>
+      <c r="CJ15" s="20"/>
       <c r="CK15" s="20"/>
       <c r="CL15" s="20"/>
-      <c r="CM15" s="20"/>
-      <c r="CN15" s="20"/>
-      <c r="CO15" s="20"/>
-      <c r="CP15" s="20"/>
+      <c r="CM15" s="12"/>
+      <c r="CN15" s="13"/>
+      <c r="CO15" s="12"/>
+      <c r="CP15" s="12"/>
       <c r="CQ15" s="12"/>
-      <c r="CR15" s="13"/>
-      <c r="CS15" s="12"/>
-      <c r="CT15" s="12"/>
-      <c r="CU15" s="13"/>
+      <c r="CR15" s="12"/>
+      <c r="CS15" s="20"/>
+      <c r="CT15" s="13"/>
+      <c r="CU15" s="12"/>
       <c r="CV15" s="12"/>
       <c r="CW15" s="12"/>
       <c r="CX15" s="12"/>
@@ -6665,8 +6990,7 @@
       <c r="CZ15" s="12"/>
       <c r="DA15" s="12"/>
       <c r="DB15" s="12"/>
-      <c r="DC15" s="12"/>
-      <c r="DD15" s="26"/>
+      <c r="DC15" s="26"/>
     </row>
     <row r="16" spans="1:108" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
@@ -6754,20 +7078,20 @@
       <c r="CE16" s="15"/>
       <c r="CF16" s="15"/>
       <c r="CG16" s="15"/>
-      <c r="CH16" s="15"/>
-      <c r="CI16" s="15"/>
-      <c r="CJ16" s="15"/>
+      <c r="CH16" s="27"/>
+      <c r="CI16" s="27"/>
+      <c r="CJ16" s="27"/>
       <c r="CK16" s="27"/>
       <c r="CL16" s="27"/>
-      <c r="CM16" s="27"/>
-      <c r="CN16" s="27"/>
-      <c r="CO16" s="27"/>
-      <c r="CP16" s="27"/>
+      <c r="CM16" s="15"/>
+      <c r="CN16" s="28"/>
+      <c r="CO16" s="15"/>
+      <c r="CP16" s="15"/>
       <c r="CQ16" s="15"/>
-      <c r="CR16" s="28"/>
-      <c r="CS16" s="15"/>
-      <c r="CT16" s="15"/>
-      <c r="CU16" s="28"/>
+      <c r="CR16" s="15"/>
+      <c r="CS16" s="27"/>
+      <c r="CT16" s="28"/>
+      <c r="CU16" s="15"/>
       <c r="CV16" s="15"/>
       <c r="CW16" s="15"/>
       <c r="CX16" s="15"/>
@@ -6775,22 +7099,22 @@
       <c r="CZ16" s="15"/>
       <c r="DA16" s="15"/>
       <c r="DB16" s="15"/>
-      <c r="DC16" s="15"/>
-      <c r="DD16" s="29"/>
+      <c r="DC16" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A7:A16"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="W4" r:id="rId1" xr:uid="{83B22828-F04D-4DFF-B34C-445B5BCB96C4}"/>
-    <hyperlink ref="X4" r:id="rId2" xr:uid="{7B954FF4-8543-47AA-A9CC-41F36163A9B1}"/>
-    <hyperlink ref="BS4" r:id="rId3" xr:uid="{4E97B430-165D-4F9F-B813-1D0DE65FB3F5}"/>
-    <hyperlink ref="BV5" r:id="rId4" xr:uid="{09758CE1-B350-40B3-88EA-F9B220FA6452}"/>
-    <hyperlink ref="BW5" r:id="rId5" xr:uid="{7C76F2D1-8C40-4440-80A1-847EAE0530DF}"/>
-    <hyperlink ref="BX5" r:id="rId6" xr:uid="{814A2D6F-8C12-499A-91E7-BF229C5BC847}"/>
+    <hyperlink ref="AY4" r:id="rId1" xr:uid="{83B22828-F04D-4DFF-B34C-445B5BCB96C4}"/>
+    <hyperlink ref="AZ4" r:id="rId2" xr:uid="{7B954FF4-8543-47AA-A9CC-41F36163A9B1}"/>
+    <hyperlink ref="BG4" r:id="rId3" xr:uid="{4E97B430-165D-4F9F-B813-1D0DE65FB3F5}"/>
+    <hyperlink ref="BL5" r:id="rId4" xr:uid="{09758CE1-B350-40B3-88EA-F9B220FA6452}"/>
+    <hyperlink ref="BM5" r:id="rId5" xr:uid="{7C76F2D1-8C40-4440-80A1-847EAE0530DF}"/>
+    <hyperlink ref="BN5" r:id="rId6" xr:uid="{814A2D6F-8C12-499A-91E7-BF229C5BC847}"/>
+    <hyperlink ref="CQ5" r:id="rId7" xr:uid="{0C1F6FFF-5DF5-4D67-930F-0182483B4E1C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Addresss format to line^city^county^postalCode^state^country
</commit_message>
<xml_diff>
--- a/src/resources/Fhir_Cohort_Import_Template.xlsx
+++ b/src/resources/Fhir_Cohort_Import_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\T21_Connectathon_Sets\Fhir_CohortPython_Generation\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCB43C2-0DF7-4B58-BFC2-A4DCE4C2982F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E559D7E-615E-471A-9B13-B24F61D73FAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8196" activeTab="4" xr2:uid="{B7CAF98F-F4CF-4673-A736-BDE9BA8D985C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8196" xr2:uid="{B7CAF98F-F4CF-4673-A736-BDE9BA8D985C}"/>
   </bookViews>
   <sheets>
     <sheet name="How To Use This Workbook" sheetId="6" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="341">
   <si>
     <t>How To Use This Workbook</t>
   </si>
@@ -175,9 +175,6 @@
     <t>Address</t>
   </si>
   <si>
-    <t>line,city,county^postalcode^state^country</t>
-  </si>
-  <si>
     <t>Entity Name</t>
   </si>
   <si>
@@ -1052,9 +1049,6 @@
     <t>http://loinc.org^8839-3^Oxygen Saturation</t>
   </si>
   <si>
-    <t>49 Meadow St, Travals, Mounds^OK^74047^US</t>
-  </si>
-  <si>
     <t>Example</t>
   </si>
   <si>
@@ -1131,6 +1125,18 @@
   </si>
   <si>
     <t>final</t>
+  </si>
+  <si>
+    <t>line^city^county^postalcode^state^country</t>
+  </si>
+  <si>
+    <t>3300 Washtenaw Avenue Suite 227^Amherst^Erie^01002^MA^USA</t>
+  </si>
+  <si>
+    <t>value^unit</t>
+  </si>
+  <si>
+    <t>35^mg</t>
   </si>
 </sst>
 </file>
@@ -1334,7 +1340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1698,6 +1704,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1707,7 +1724,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1930,26 +1947,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1962,8 +1971,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2374,174 +2401,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC3792E-0A86-43B6-8F3D-128E7961060A}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="113.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="46.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="96.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="46.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:3" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
-    </row>
-    <row r="2" spans="1:3" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="102" t="s">
+      <c r="B1" s="106"/>
+    </row>
+    <row r="2" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
     </row>
     <row r="3" spans="1:3" ht="103.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="104" t="s">
+      <c r="A3" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="104"/>
-    </row>
-    <row r="4" spans="1:3" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="103" t="s">
+      <c r="B3" s="101"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="103"/>
-      <c r="C4" s="103"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="108"/>
     </row>
     <row r="5" spans="1:3" ht="40.799999999999997" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="107"/>
-    </row>
-    <row r="6" spans="1:3" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="B5" s="103"/>
+    </row>
+    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="109" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="97" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="109" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="97" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="109" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="97" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="109" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="97" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="102" t="s">
+    <row r="10" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="102"/>
-      <c r="C10" s="102"/>
+      <c r="B10" s="107"/>
+      <c r="C10" s="107"/>
     </row>
     <row r="11" spans="1:3" ht="37.200000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="104" t="s">
-        <v>306</v>
-      </c>
-      <c r="B11" s="104"/>
+      <c r="A11" s="101" t="s">
+        <v>305</v>
+      </c>
+      <c r="B11" s="101"/>
     </row>
     <row r="12" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="106" t="s">
+      <c r="A12" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="106"/>
+      <c r="B12" s="102"/>
     </row>
     <row r="13" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="106" t="s">
+      <c r="A13" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="106"/>
+      <c r="B13" s="102"/>
     </row>
     <row r="14" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="106" t="s">
-        <v>309</v>
-      </c>
-      <c r="B14" s="106"/>
-    </row>
-    <row r="15" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="101" t="s">
+      <c r="A14" s="102" t="s">
+        <v>308</v>
+      </c>
+      <c r="B14" s="102"/>
+    </row>
+    <row r="15" spans="1:3" ht="34.799999999999997" x14ac:dyDescent="0.35">
+      <c r="A15" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="101"/>
-      <c r="C15" s="101" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="98" t="s">
+      <c r="B15" s="110"/>
+      <c r="C15" s="110" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="111" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="98" t="s">
+      <c r="C16" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="111" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="98" t="s">
+      <c r="C17" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="111" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="97" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" t="s">
-        <v>312</v>
+        <v>337</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="111" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A6" location="ResourceDefinitions!A1" display="ResourceDefinitions" xr:uid="{97DCBFA9-D76D-4D75-AF15-2C90B1F524D6}"/>
-    <hyperlink ref="A7" location="ResourceLinks!A1" display="ResourceLinks" xr:uid="{16D1013F-4A78-4D8A-95CF-EDDDBE87F520}"/>
-    <hyperlink ref="A8" location="PatientData!A1" display="PatientData" xr:uid="{58703038-E3F4-4A0B-8C43-AD41E4DEF7A4}"/>
-    <hyperlink ref="A9" location="ReferenceSheet!A1" display="ReferenceSheet" xr:uid="{12FA169C-4EC7-423A-BB5A-0CFA46D0ED89}"/>
+    <hyperlink ref="A6" location="ResourceDefinitions!A1" display="ResourceDefinitions" xr:uid="{21E4973D-DCF1-4F08-A5DE-B12BC88A3D35}"/>
+    <hyperlink ref="A7" location="ResourceLinks!A1" display="ResourceLinks" xr:uid="{1EBB1C90-EB28-4AA5-B6B2-161B7B81826B}"/>
+    <hyperlink ref="A8" location="PatientData!A1" display="PatientData" xr:uid="{6B6730B2-22DC-414E-899D-F7F911BAF8E7}"/>
+    <hyperlink ref="A9" location="ReferenceSheet!A1" display="ReferenceSheet" xr:uid="{16BB53CA-8F79-4723-8B26-2C56914397A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2563,25 +2602,25 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="98" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="99" t="s">
-        <v>307</v>
-      </c>
-      <c r="B2" s="100" t="s">
+      <c r="C2" s="98" t="s">
         <v>24</v>
-      </c>
-      <c r="C2" s="99" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2653,24 +2692,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2704,10 +2743,10 @@
   <sheetData>
     <row r="1" spans="1:127" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -2837,10 +2876,10 @@
     </row>
     <row r="2" spans="1:127" s="2" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>35</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -2970,10 +3009,10 @@
     </row>
     <row r="3" spans="1:127" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="32" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>37</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -3103,10 +3142,10 @@
     </row>
     <row r="4" spans="1:127" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="35" t="s">
         <v>38</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>39</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3236,10 +3275,10 @@
     </row>
     <row r="5" spans="1:127" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>40</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>41</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
@@ -3369,10 +3408,10 @@
     </row>
     <row r="6" spans="1:127" s="2" customFormat="1" ht="52.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="37" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>43</v>
       </c>
       <c r="C6" s="90"/>
       <c r="D6" s="91"/>
@@ -3501,7 +3540,7 @@
       <c r="DW6" s="15"/>
     </row>
     <row r="7" spans="1:127" x14ac:dyDescent="0.3">
-      <c r="A7" s="108"/>
+      <c r="A7" s="104"/>
       <c r="B7" s="26"/>
       <c r="C7" s="17"/>
       <c r="D7" s="18"/>
@@ -3611,7 +3650,7 @@
       <c r="DD7" s="20"/>
     </row>
     <row r="8" spans="1:127" x14ac:dyDescent="0.3">
-      <c r="A8" s="108"/>
+      <c r="A8" s="104"/>
       <c r="B8" s="5"/>
       <c r="C8" s="21"/>
       <c r="D8" s="8"/>
@@ -3721,7 +3760,7 @@
       <c r="DD8" s="22"/>
     </row>
     <row r="9" spans="1:127" x14ac:dyDescent="0.3">
-      <c r="A9" s="108"/>
+      <c r="A9" s="104"/>
       <c r="B9" s="5"/>
       <c r="C9" s="21"/>
       <c r="D9" s="8"/>
@@ -3831,7 +3870,7 @@
       <c r="DD9" s="22"/>
     </row>
     <row r="10" spans="1:127" x14ac:dyDescent="0.3">
-      <c r="A10" s="108"/>
+      <c r="A10" s="104"/>
       <c r="B10" s="5"/>
       <c r="C10" s="21"/>
       <c r="D10" s="8"/>
@@ -3941,7 +3980,7 @@
       <c r="DD10" s="22"/>
     </row>
     <row r="11" spans="1:127" x14ac:dyDescent="0.3">
-      <c r="A11" s="108"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="5"/>
       <c r="C11" s="21"/>
       <c r="D11" s="8"/>
@@ -4051,7 +4090,7 @@
       <c r="DD11" s="22"/>
     </row>
     <row r="12" spans="1:127" x14ac:dyDescent="0.3">
-      <c r="A12" s="108"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="5"/>
       <c r="C12" s="21"/>
       <c r="D12" s="8"/>
@@ -4161,7 +4200,7 @@
       <c r="DD12" s="22"/>
     </row>
     <row r="13" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="108"/>
+      <c r="A13" s="104"/>
       <c r="B13" s="5"/>
       <c r="C13" s="21"/>
       <c r="D13" s="8"/>
@@ -4271,7 +4310,7 @@
       <c r="DD13" s="22"/>
     </row>
     <row r="14" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="108"/>
+      <c r="A14" s="104"/>
       <c r="B14" s="5"/>
       <c r="C14" s="21"/>
       <c r="D14" s="8"/>
@@ -4381,7 +4420,7 @@
       <c r="DD14" s="22"/>
     </row>
     <row r="15" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="108"/>
+      <c r="A15" s="104"/>
       <c r="B15" s="5"/>
       <c r="C15" s="21"/>
       <c r="D15" s="8"/>
@@ -4491,7 +4530,7 @@
       <c r="DD15" s="22"/>
     </row>
     <row r="16" spans="1:127" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="109"/>
+      <c r="A16" s="105"/>
       <c r="B16" s="6"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
@@ -4613,9 +4652,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D010D53-A2B8-4D7D-8239-2883E618B035}">
   <dimension ref="A1:DR16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N9" sqref="N9"/>
+      <selection pane="topRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4633,10 +4672,10 @@
   <sheetData>
     <row r="1" spans="1:122" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>32</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>33</v>
       </c>
       <c r="C1" s="72"/>
       <c r="D1" s="73"/>
@@ -4761,427 +4800,427 @@
     </row>
     <row r="2" spans="1:122" s="2" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>35</v>
-      </c>
       <c r="C2" s="89" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="E2" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="F2" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="G2" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="H2" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="I2" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="J2" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="K2" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="L2" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="M2" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="N2" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="O2" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="P2" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="P2" s="38" t="s">
+      <c r="Q2" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="Q2" s="38" t="s">
+      <c r="R2" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="R2" s="38" t="s">
+      <c r="S2" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="S2" s="38" t="s">
+      <c r="T2" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="T2" s="38" t="s">
+      <c r="U2" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="W2" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="U2" s="38" t="s">
+      <c r="X2" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y2" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="V2" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="W2" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="X2" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y2" s="40" t="s">
+      <c r="Z2" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="Z2" s="40" t="s">
+      <c r="AA2" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="AA2" s="40" t="s">
+      <c r="AB2" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="AB2" s="40" t="s">
+      <c r="AC2" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="AC2" s="42" t="s">
+      <c r="AD2" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="AD2" s="42" t="s">
+      <c r="AE2" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="AE2" s="42" t="s">
+      <c r="AF2" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="AF2" s="44" t="s">
+      <c r="AG2" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AH2" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="AH2" s="44" t="s">
+      <c r="AI2" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AI2" s="44" t="s">
+      <c r="AJ2" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="AJ2" s="44" t="s">
+      <c r="AK2" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="AK2" s="46" t="s">
+      <c r="AL2" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="AL2" s="46" t="s">
+      <c r="AM2" s="46" t="s">
+        <v>312</v>
+      </c>
+      <c r="AN2" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="AM2" s="46" t="s">
+      <c r="AO2" s="46" t="s">
+        <v>313</v>
+      </c>
+      <c r="AP2" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ2" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR2" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS2" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT2" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU2" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="AV2" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW2" s="48" t="s">
         <v>314</v>
       </c>
-      <c r="AN2" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO2" s="46" t="s">
+      <c r="AX2" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="AY2" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="AZ2" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="BA2" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="BB2" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="BC2" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="AP2" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="AQ2" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="AR2" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="AS2" s="48" t="s">
-        <v>82</v>
-      </c>
-      <c r="AT2" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="AU2" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="AV2" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="AW2" s="48" t="s">
+      <c r="BD2" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="BE2" s="50" t="s">
         <v>316</v>
       </c>
-      <c r="AX2" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="AY2" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="AZ2" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="BA2" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="BB2" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="BC2" s="50" t="s">
+      <c r="BF2" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="BG2" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="BH2" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="BI2" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="BJ2" s="52" t="s">
         <v>317</v>
       </c>
-      <c r="BD2" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE2" s="50" t="s">
+      <c r="BK2" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="BL2" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="BM2" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="BN2" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="BO2" s="56" t="s">
         <v>318</v>
       </c>
-      <c r="BF2" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="BG2" s="52" t="s">
-        <v>93</v>
-      </c>
-      <c r="BH2" s="52" t="s">
-        <v>94</v>
-      </c>
-      <c r="BI2" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="BJ2" s="52" t="s">
+      <c r="BP2" s="56" t="s">
         <v>319</v>
       </c>
-      <c r="BK2" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="BL2" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="BM2" s="54" t="s">
+      <c r="BQ2" s="56" t="s">
+        <v>320</v>
+      </c>
+      <c r="BR2" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="BS2" s="56" t="s">
+        <v>321</v>
+      </c>
+      <c r="BT2" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="BU2" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="BN2" s="56" t="s">
+      <c r="BV2" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="BW2" s="58" t="s">
+        <v>320</v>
+      </c>
+      <c r="BX2" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="BO2" s="56" t="s">
-        <v>320</v>
-      </c>
-      <c r="BP2" s="56" t="s">
-        <v>321</v>
-      </c>
-      <c r="BQ2" s="56" t="s">
-        <v>322</v>
-      </c>
-      <c r="BR2" s="56" t="s">
+      <c r="BY2" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="BZ2" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="CA2" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="CB2" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="CC2" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="CD2" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="CE2" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="CF2" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="CG2" s="62" t="s">
+        <v>323</v>
+      </c>
+      <c r="CH2" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="CI2" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="BS2" s="56" t="s">
-        <v>323</v>
-      </c>
-      <c r="BT2" s="56" t="s">
-        <v>324</v>
-      </c>
-      <c r="BU2" s="58" t="s">
-        <v>99</v>
-      </c>
-      <c r="BV2" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="BW2" s="58" t="s">
-        <v>322</v>
-      </c>
-      <c r="BX2" s="58" t="s">
+      <c r="CJ2" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="CK2" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="CL2" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="CM2" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="CN2" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="CO2" s="66" t="s">
+        <v>122</v>
+      </c>
+      <c r="CP2" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="CQ2" s="66" t="s">
+        <v>124</v>
+      </c>
+      <c r="CR2" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="CS2" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="CT2" s="68" t="s">
+        <v>107</v>
+      </c>
+      <c r="CU2" s="68" t="s">
+        <v>107</v>
+      </c>
+      <c r="CV2" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="CW2" s="70" t="s">
+        <v>127</v>
+      </c>
+      <c r="CX2" s="70" t="s">
+        <v>128</v>
+      </c>
+      <c r="CY2" s="70" t="s">
+        <v>129</v>
+      </c>
+      <c r="CZ2" s="70" t="s">
+        <v>130</v>
+      </c>
+      <c r="DA2" s="70" t="s">
+        <v>131</v>
+      </c>
+      <c r="DB2" s="70" t="s">
+        <v>132</v>
+      </c>
+      <c r="DC2" s="70" t="s">
+        <v>133</v>
+      </c>
+      <c r="DD2" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="DE2" s="70" t="s">
+        <v>135</v>
+      </c>
+      <c r="DF2" s="93" t="s">
+        <v>105</v>
+      </c>
+      <c r="DG2" s="93" t="s">
+        <v>136</v>
+      </c>
+      <c r="DH2" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="DI2" s="93" t="s">
         <v>100</v>
       </c>
-      <c r="BY2" s="58" t="s">
-        <v>107</v>
-      </c>
-      <c r="BZ2" s="58" t="s">
-        <v>101</v>
-      </c>
-      <c r="CA2" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="CB2" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="CC2" s="60" t="s">
-        <v>104</v>
-      </c>
-      <c r="CD2" s="61" t="s">
-        <v>105</v>
-      </c>
-      <c r="CE2" s="62" t="s">
-        <v>99</v>
-      </c>
-      <c r="CF2" s="62" t="s">
-        <v>106</v>
-      </c>
-      <c r="CG2" s="62" t="s">
-        <v>325</v>
-      </c>
-      <c r="CH2" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="CI2" s="62" t="s">
+      <c r="DJ2" s="93" t="s">
         <v>108</v>
       </c>
-      <c r="CJ2" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="CK2" s="64" t="s">
-        <v>119</v>
-      </c>
-      <c r="CL2" s="64" t="s">
-        <v>120</v>
-      </c>
-      <c r="CM2" s="64" t="s">
-        <v>121</v>
-      </c>
-      <c r="CN2" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="CO2" s="66" t="s">
-        <v>123</v>
-      </c>
-      <c r="CP2" s="66" t="s">
-        <v>124</v>
-      </c>
-      <c r="CQ2" s="66" t="s">
-        <v>125</v>
-      </c>
-      <c r="CR2" s="66" t="s">
-        <v>126</v>
-      </c>
-      <c r="CS2" s="68" t="s">
-        <v>99</v>
-      </c>
-      <c r="CT2" s="68" t="s">
-        <v>108</v>
-      </c>
-      <c r="CU2" s="68" t="s">
-        <v>108</v>
-      </c>
-      <c r="CV2" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="CW2" s="70" t="s">
-        <v>128</v>
-      </c>
-      <c r="CX2" s="70" t="s">
-        <v>129</v>
-      </c>
-      <c r="CY2" s="70" t="s">
-        <v>130</v>
-      </c>
-      <c r="CZ2" s="70" t="s">
-        <v>131</v>
-      </c>
-      <c r="DA2" s="70" t="s">
-        <v>132</v>
-      </c>
-      <c r="DB2" s="70" t="s">
-        <v>133</v>
-      </c>
-      <c r="DC2" s="70" t="s">
-        <v>134</v>
-      </c>
-      <c r="DD2" s="70" t="s">
-        <v>135</v>
-      </c>
-      <c r="DE2" s="70" t="s">
-        <v>136</v>
-      </c>
-      <c r="DF2" s="93" t="s">
-        <v>106</v>
-      </c>
-      <c r="DG2" s="93" t="s">
-        <v>137</v>
-      </c>
-      <c r="DH2" s="93" t="s">
-        <v>108</v>
-      </c>
-      <c r="DI2" s="93" t="s">
-        <v>101</v>
-      </c>
-      <c r="DJ2" s="93" t="s">
+      <c r="DK2" s="93" t="s">
         <v>109</v>
       </c>
-      <c r="DK2" s="93" t="s">
+      <c r="DL2" s="93" t="s">
         <v>110</v>
       </c>
-      <c r="DL2" s="93" t="s">
+      <c r="DM2" s="93" t="s">
         <v>111</v>
       </c>
-      <c r="DM2" s="93" t="s">
+      <c r="DN2" s="93" t="s">
         <v>112</v>
       </c>
-      <c r="DN2" s="93" t="s">
+      <c r="DO2" s="93" t="s">
         <v>113</v>
       </c>
-      <c r="DO2" s="93" t="s">
+      <c r="DP2" s="93" t="s">
         <v>114</v>
       </c>
-      <c r="DP2" s="93" t="s">
+      <c r="DQ2" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="DQ2" s="93" t="s">
+      <c r="DR2" s="93" t="s">
         <v>116</v>
-      </c>
-      <c r="DR2" s="93" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:122" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="32" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>37</v>
       </c>
       <c r="C3" s="89"/>
       <c r="D3" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="G3" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="H3" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="J3" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="K3" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="L3" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="H3" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="I3" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="J3" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="K3" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="L3" s="38" t="s">
+      <c r="M3" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="O3" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="P3" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q3" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="R3" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="S3" s="38" t="s">
         <v>140</v>
-      </c>
-      <c r="M3" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="N3" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="O3" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="P3" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q3" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="R3" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="S3" s="38" t="s">
-        <v>141</v>
       </c>
       <c r="T3" s="38" t="s">
         <v>19</v>
@@ -5205,49 +5244,49 @@
         <v>16</v>
       </c>
       <c r="AA3" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB3" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC3" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD3" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="AB3" s="40" t="s">
+      <c r="AE3" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="AC3" s="42" t="s">
-        <v>139</v>
-      </c>
-      <c r="AD3" s="42" t="s">
-        <v>140</v>
-      </c>
-      <c r="AE3" s="42" t="s">
-        <v>140</v>
-      </c>
       <c r="AF3" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG3" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="AG3" s="44" t="s">
-        <v>139</v>
-      </c>
       <c r="AH3" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI3" s="44" t="s">
         <v>138</v>
-      </c>
-      <c r="AI3" s="44" t="s">
-        <v>139</v>
       </c>
       <c r="AJ3" s="44" t="s">
         <v>19</v>
       </c>
       <c r="AK3" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AL3" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AM3" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN3" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="AN3" s="46" t="s">
-        <v>139</v>
-      </c>
       <c r="AO3" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AP3" s="46" t="s">
         <v>19</v>
@@ -5255,13 +5294,13 @@
       <c r="AQ3" s="46"/>
       <c r="AR3" s="46"/>
       <c r="AS3" s="48" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AT3" s="48" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AU3" s="48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AV3" s="48" t="s">
         <v>18</v>
@@ -5270,10 +5309,10 @@
         <v>16</v>
       </c>
       <c r="AX3" s="48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AY3" s="48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AZ3" s="48" t="s">
         <v>16</v>
@@ -5282,7 +5321,7 @@
         <v>16</v>
       </c>
       <c r="BB3" s="50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BC3" s="50" t="s">
         <v>16</v>
@@ -5291,10 +5330,10 @@
         <v>16</v>
       </c>
       <c r="BE3" s="50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BF3" s="50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BG3" s="52" t="s">
         <v>16</v>
@@ -5309,16 +5348,16 @@
         <v>16</v>
       </c>
       <c r="BK3" s="54" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BL3" s="54" t="s">
         <v>16</v>
       </c>
       <c r="BM3" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="BN3" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="BN3" s="56" t="s">
-        <v>144</v>
       </c>
       <c r="BO3" s="56" t="s">
         <v>18</v>
@@ -5330,16 +5369,16 @@
         <v>16</v>
       </c>
       <c r="BR3" s="56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BS3" s="56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BT3" s="56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BU3" s="58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BV3" s="58" t="s">
         <v>16</v>
@@ -5348,28 +5387,28 @@
         <v>16</v>
       </c>
       <c r="BX3" s="58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="BY3" s="58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BZ3" s="58" t="s">
         <v>16</v>
       </c>
       <c r="CA3" s="60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CB3" s="60" t="s">
         <v>16</v>
       </c>
       <c r="CC3" s="60" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="CD3" s="61" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="CE3" s="62" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CF3" s="62" t="s">
         <v>16</v>
@@ -5378,10 +5417,10 @@
         <v>16</v>
       </c>
       <c r="CH3" s="62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="CI3" s="62" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="CJ3" s="64" t="s">
         <v>16</v>
@@ -5396,55 +5435,55 @@
         <v>16</v>
       </c>
       <c r="CN3" s="64" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="CO3" s="66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CP3" s="66" t="s">
         <v>16</v>
       </c>
       <c r="CQ3" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="CR3" s="66" t="s">
+        <v>138</v>
+      </c>
+      <c r="CS3" s="68" t="s">
+        <v>137</v>
+      </c>
+      <c r="CT3" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="CU3" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="CV3" s="68" t="s">
         <v>143</v>
       </c>
-      <c r="CR3" s="66" t="s">
-        <v>139</v>
-      </c>
-      <c r="CS3" s="68" t="s">
+      <c r="CW3" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="CT3" s="68" t="s">
-        <v>146</v>
-      </c>
-      <c r="CU3" s="68" t="s">
-        <v>146</v>
-      </c>
-      <c r="CV3" s="68" t="s">
-        <v>144</v>
-      </c>
-      <c r="CW3" s="70" t="s">
-        <v>139</v>
-      </c>
       <c r="CX3" s="70" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="CY3" s="70" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="CZ3" s="70" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="DA3" s="70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="DB3" s="70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="DC3" s="70" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="DD3" s="70" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="DE3" s="70" t="s">
         <v>16</v>
@@ -5453,37 +5492,37 @@
         <v>16</v>
       </c>
       <c r="DG3" s="93" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="DH3" s="93" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="DI3" s="93" t="s">
         <v>16</v>
       </c>
       <c r="DJ3" s="93" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="DK3" s="93" t="s">
+        <v>141</v>
+      </c>
+      <c r="DL3" s="93" t="s">
+        <v>146</v>
+      </c>
+      <c r="DM3" s="93" t="s">
+        <v>147</v>
+      </c>
+      <c r="DN3" s="93" t="s">
+        <v>148</v>
+      </c>
+      <c r="DO3" s="93" t="s">
+        <v>149</v>
+      </c>
+      <c r="DP3" s="93" t="s">
         <v>142</v>
       </c>
-      <c r="DL3" s="93" t="s">
-        <v>147</v>
-      </c>
-      <c r="DM3" s="93" t="s">
-        <v>148</v>
-      </c>
-      <c r="DN3" s="93" t="s">
-        <v>149</v>
-      </c>
-      <c r="DO3" s="93" t="s">
+      <c r="DQ3" s="93" t="s">
         <v>150</v>
-      </c>
-      <c r="DP3" s="93" t="s">
-        <v>143</v>
-      </c>
-      <c r="DQ3" s="93" t="s">
-        <v>151</v>
       </c>
       <c r="DR3" s="93" t="s">
         <v>16</v>
@@ -5491,19 +5530,19 @@
     </row>
     <row r="4" spans="1:122" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="35" t="s">
-        <v>39</v>
-      </c>
       <c r="C4" s="94" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="E4" s="38" t="s">
         <v>155</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>156</v>
       </c>
       <c r="F4" s="38"/>
       <c r="G4" s="38"/>
@@ -5515,14 +5554,14 @@
       <c r="M4" s="38"/>
       <c r="N4" s="38"/>
       <c r="O4" s="38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P4" s="38"/>
       <c r="Q4" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="R4" s="38" t="s">
         <v>158</v>
-      </c>
-      <c r="R4" s="38" t="s">
-        <v>159</v>
       </c>
       <c r="S4" s="39"/>
       <c r="T4" s="39"/>
@@ -5531,35 +5570,35 @@
       <c r="W4" s="39"/>
       <c r="X4" s="39"/>
       <c r="Y4" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z4" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="Z4" s="41" t="s">
-        <v>161</v>
-      </c>
       <c r="AA4" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AB4" s="40"/>
       <c r="AC4" s="43"/>
       <c r="AD4" s="43"/>
       <c r="AE4" s="43"/>
       <c r="AF4" s="45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG4" s="45"/>
       <c r="AH4" s="44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AI4" s="44"/>
       <c r="AJ4" s="45"/>
       <c r="AK4" s="47"/>
       <c r="AL4" s="47"/>
       <c r="AM4" s="46" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="AN4" s="46"/>
       <c r="AO4" s="46" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AP4" s="47"/>
       <c r="AQ4" s="47"/>
@@ -5567,114 +5606,114 @@
       <c r="AS4" s="49"/>
       <c r="AT4" s="49"/>
       <c r="AU4" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="AV4" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="AV4" s="49" t="s">
+      <c r="AW4" s="49" t="s">
         <v>164</v>
-      </c>
-      <c r="AW4" s="49" t="s">
-        <v>165</v>
       </c>
       <c r="AX4" s="49"/>
       <c r="AY4" s="49"/>
       <c r="AZ4" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="BA4" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="BA4" s="49" t="s">
+      <c r="BB4" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="BB4" s="51" t="s">
+      <c r="BC4" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="BC4" s="51" t="s">
+      <c r="BD4" s="51" t="s">
         <v>169</v>
-      </c>
-      <c r="BD4" s="51" t="s">
-        <v>170</v>
       </c>
       <c r="BE4" s="51"/>
       <c r="BF4" s="51"/>
       <c r="BG4" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="BH4" s="53" t="s">
         <v>171</v>
       </c>
-      <c r="BH4" s="53" t="s">
+      <c r="BI4" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="BI4" s="53" t="s">
+      <c r="BJ4" s="53" t="s">
         <v>173</v>
       </c>
-      <c r="BJ4" s="53" t="s">
+      <c r="BK4" s="55" t="s">
         <v>174</v>
       </c>
-      <c r="BK4" s="55" t="s">
+      <c r="BL4" s="55" t="s">
         <v>175</v>
-      </c>
-      <c r="BL4" s="55" t="s">
-        <v>176</v>
       </c>
       <c r="BM4" s="55"/>
       <c r="BN4" s="57"/>
       <c r="BO4" s="57" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BP4" s="57" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BQ4" s="57" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="BR4" s="57"/>
       <c r="BS4" s="57"/>
       <c r="BT4" s="57"/>
       <c r="BU4" s="59" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BV4" s="59" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BW4" s="59" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="BX4" s="59"/>
       <c r="BY4" s="59"/>
       <c r="BZ4" s="59" t="s">
+        <v>177</v>
+      </c>
+      <c r="CA4" s="61" t="s">
         <v>178</v>
       </c>
-      <c r="CA4" s="61" t="s">
+      <c r="CB4" s="61" t="s">
         <v>179</v>
-      </c>
-      <c r="CB4" s="61" t="s">
-        <v>180</v>
       </c>
       <c r="CC4" s="61"/>
       <c r="CD4" s="61"/>
       <c r="CE4" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="CF4" s="63" t="s">
         <v>181</v>
       </c>
-      <c r="CF4" s="63" t="s">
-        <v>182</v>
-      </c>
       <c r="CG4" s="63" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="CH4" s="62"/>
       <c r="CI4" s="62"/>
       <c r="CJ4" s="65" t="s">
+        <v>182</v>
+      </c>
+      <c r="CK4" s="65" t="s">
         <v>183</v>
       </c>
-      <c r="CK4" s="65" t="s">
+      <c r="CL4" s="65" t="s">
         <v>184</v>
-      </c>
-      <c r="CL4" s="65" t="s">
-        <v>185</v>
       </c>
       <c r="CM4" s="65"/>
       <c r="CN4" s="65"/>
       <c r="CO4" s="67" t="s">
+        <v>185</v>
+      </c>
+      <c r="CP4" s="67" t="s">
         <v>186</v>
-      </c>
-      <c r="CP4" s="67" t="s">
-        <v>187</v>
       </c>
       <c r="CQ4" s="66"/>
       <c r="CR4" s="66"/>
@@ -5691,10 +5730,10 @@
       <c r="DC4" s="71"/>
       <c r="DD4" s="71"/>
       <c r="DE4" s="71" t="s">
+        <v>187</v>
+      </c>
+      <c r="DF4" s="93" t="s">
         <v>188</v>
-      </c>
-      <c r="DF4" s="93" t="s">
-        <v>189</v>
       </c>
       <c r="DG4" s="93"/>
       <c r="DH4" s="93"/>
@@ -5711,732 +5750,732 @@
     </row>
     <row r="5" spans="1:122" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="30" t="s">
-        <v>41</v>
-      </c>
       <c r="C5" s="94" t="s">
+        <v>189</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="L5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="M5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="N5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="O5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="P5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="R5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="S5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="T5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="U5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="V5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="W5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="X5" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y5" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="Z5" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="AA5" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="AB5" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="G5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="I5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="J5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="K5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="L5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="M5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="N5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="O5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="P5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="R5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="S5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="T5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="U5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="V5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="W5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="X5" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="Y5" s="40" t="s">
+      <c r="AC5" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="Z5" s="40" t="s">
+      <c r="AD5" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="AA5" s="40" t="s">
+      <c r="AE5" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="AB5" s="40" t="s">
-        <v>191</v>
-      </c>
-      <c r="AC5" s="42" t="s">
+      <c r="AF5" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="AD5" s="42" t="s">
+      <c r="AG5" s="44" t="s">
         <v>192</v>
       </c>
-      <c r="AE5" s="42" t="s">
+      <c r="AH5" s="44" t="s">
         <v>192</v>
       </c>
-      <c r="AF5" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="AG5" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="AH5" s="44" t="s">
-        <v>193</v>
-      </c>
       <c r="AI5" s="44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AJ5" s="44"/>
       <c r="AK5" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="AL5" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="AM5" s="47" t="s">
+        <v>193</v>
+      </c>
+      <c r="AN5" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="AO5" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="AP5" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="AQ5" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="AR5" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="AS5" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="AL5" s="46" t="s">
+      <c r="AT5" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="AM5" s="47" t="s">
+      <c r="AU5" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="AN5" s="46" t="s">
+      <c r="AV5" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="AO5" s="46" t="s">
+      <c r="AW5" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="AP5" s="46" t="s">
+      <c r="AX5" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="AQ5" s="46" t="s">
+      <c r="AY5" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="AR5" s="46" t="s">
+      <c r="AZ5" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="AS5" s="48" t="s">
+      <c r="BA5" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="BB5" s="51" t="s">
         <v>195</v>
       </c>
-      <c r="AT5" s="48" t="s">
+      <c r="BC5" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="AU5" s="48" t="s">
+      <c r="BD5" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="AV5" s="48" t="s">
+      <c r="BE5" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="AW5" s="48" t="s">
+      <c r="BF5" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="AX5" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="AY5" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="AZ5" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="BA5" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="BB5" s="51" t="s">
+      <c r="BG5" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="BC5" s="50" t="s">
+      <c r="BH5" s="52" t="s">
         <v>196</v>
       </c>
-      <c r="BD5" s="50" t="s">
+      <c r="BI5" s="52" t="s">
         <v>196</v>
-      </c>
-      <c r="BE5" s="50" t="s">
-        <v>196</v>
-      </c>
-      <c r="BF5" s="50" t="s">
-        <v>196</v>
-      </c>
-      <c r="BG5" s="53" t="s">
-        <v>197</v>
-      </c>
-      <c r="BH5" s="52" t="s">
-        <v>197</v>
-      </c>
-      <c r="BI5" s="52" t="s">
-        <v>197</v>
       </c>
       <c r="BJ5" s="52"/>
       <c r="BK5" s="55" t="s">
+        <v>197</v>
+      </c>
+      <c r="BL5" s="54" t="s">
+        <v>197</v>
+      </c>
+      <c r="BM5" s="54" t="s">
+        <v>197</v>
+      </c>
+      <c r="BN5" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="BL5" s="54" t="s">
+      <c r="BO5" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="BM5" s="54" t="s">
+      <c r="BP5" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="BN5" s="57" t="s">
+      <c r="BQ5" s="57" t="s">
+        <v>201</v>
+      </c>
+      <c r="BR5" s="57" t="s">
+        <v>201</v>
+      </c>
+      <c r="BS5" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="BT5" s="56" t="s">
+        <v>198</v>
+      </c>
+      <c r="BU5" s="58" t="s">
         <v>199</v>
       </c>
-      <c r="BO5" s="57" t="s">
+      <c r="BV5" s="58" t="s">
         <v>199</v>
       </c>
-      <c r="BP5" s="57" t="s">
+      <c r="BW5" s="58" t="s">
+        <v>201</v>
+      </c>
+      <c r="BX5" s="58" t="s">
         <v>199</v>
       </c>
-      <c r="BQ5" s="57" t="s">
+      <c r="BY5" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="BZ5" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="CA5" s="61" t="s">
+        <v>200</v>
+      </c>
+      <c r="CB5" s="60" t="s">
+        <v>200</v>
+      </c>
+      <c r="CC5" s="60" t="s">
+        <v>200</v>
+      </c>
+      <c r="CD5" s="61" t="s">
+        <v>200</v>
+      </c>
+      <c r="CE5" s="63" t="s">
+        <v>201</v>
+      </c>
+      <c r="CF5" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="CG5" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="CH5" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="CI5" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="CJ5" s="64" t="s">
         <v>202</v>
       </c>
-      <c r="BR5" s="57" t="s">
+      <c r="CK5" s="64" t="s">
         <v>202</v>
       </c>
-      <c r="BS5" s="57" t="s">
-        <v>199</v>
-      </c>
-      <c r="BT5" s="56" t="s">
-        <v>199</v>
-      </c>
-      <c r="BU5" s="58" t="s">
-        <v>200</v>
-      </c>
-      <c r="BV5" s="58" t="s">
-        <v>200</v>
-      </c>
-      <c r="BW5" s="58" t="s">
+      <c r="CL5" s="64" t="s">
         <v>202</v>
       </c>
-      <c r="BX5" s="58" t="s">
-        <v>200</v>
-      </c>
-      <c r="BY5" s="59" t="s">
+      <c r="CM5" s="64" t="s">
         <v>202</v>
-      </c>
-      <c r="BZ5" s="58" t="s">
-        <v>200</v>
-      </c>
-      <c r="CA5" s="61" t="s">
-        <v>201</v>
-      </c>
-      <c r="CB5" s="60" t="s">
-        <v>201</v>
-      </c>
-      <c r="CC5" s="60" t="s">
-        <v>201</v>
-      </c>
-      <c r="CD5" s="61" t="s">
-        <v>201</v>
-      </c>
-      <c r="CE5" s="63" t="s">
-        <v>202</v>
-      </c>
-      <c r="CF5" s="62" t="s">
-        <v>202</v>
-      </c>
-      <c r="CG5" s="62" t="s">
-        <v>202</v>
-      </c>
-      <c r="CH5" s="62" t="s">
-        <v>202</v>
-      </c>
-      <c r="CI5" s="62" t="s">
-        <v>202</v>
-      </c>
-      <c r="CJ5" s="64" t="s">
-        <v>203</v>
-      </c>
-      <c r="CK5" s="64" t="s">
-        <v>203</v>
-      </c>
-      <c r="CL5" s="64" t="s">
-        <v>203</v>
-      </c>
-      <c r="CM5" s="64" t="s">
-        <v>203</v>
       </c>
       <c r="CN5" s="64"/>
       <c r="CO5" s="66" t="s">
+        <v>203</v>
+      </c>
+      <c r="CP5" s="66" t="s">
+        <v>203</v>
+      </c>
+      <c r="CQ5" s="66" t="s">
+        <v>203</v>
+      </c>
+      <c r="CR5" s="66" t="s">
+        <v>203</v>
+      </c>
+      <c r="CS5" s="69" t="s">
         <v>204</v>
       </c>
-      <c r="CP5" s="66" t="s">
+      <c r="CT5" s="69" t="s">
         <v>204</v>
       </c>
-      <c r="CQ5" s="66" t="s">
+      <c r="CU5" s="68" t="s">
         <v>204</v>
       </c>
-      <c r="CR5" s="66" t="s">
-        <v>204</v>
-      </c>
-      <c r="CS5" s="69" t="s">
+      <c r="CV5" s="68" t="s">
         <v>205</v>
       </c>
-      <c r="CT5" s="69" t="s">
-        <v>205</v>
-      </c>
-      <c r="CU5" s="68" t="s">
-        <v>205</v>
-      </c>
-      <c r="CV5" s="68" t="s">
+      <c r="CW5" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="CW5" s="70" t="s">
+      <c r="CX5" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="CY5" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="CZ5" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="DA5" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="DB5" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="DC5" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="DD5" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="DE5" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="DF5" s="93" t="s">
         <v>207</v>
       </c>
-      <c r="CX5" s="70" t="s">
+      <c r="DG5" s="93" t="s">
         <v>207</v>
       </c>
-      <c r="CY5" s="70" t="s">
-        <v>207</v>
-      </c>
-      <c r="CZ5" s="70" t="s">
-        <v>207</v>
-      </c>
-      <c r="DA5" s="70" t="s">
-        <v>207</v>
-      </c>
-      <c r="DB5" s="70" t="s">
-        <v>207</v>
-      </c>
-      <c r="DC5" s="70" t="s">
-        <v>207</v>
-      </c>
-      <c r="DD5" s="70" t="s">
-        <v>207</v>
-      </c>
-      <c r="DE5" s="70" t="s">
-        <v>207</v>
-      </c>
-      <c r="DF5" s="93" t="s">
-        <v>208</v>
-      </c>
-      <c r="DG5" s="93" t="s">
-        <v>208</v>
-      </c>
       <c r="DH5" s="93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DI5" s="93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DJ5" s="93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DK5" s="93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DL5" s="93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DM5" s="93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DN5" s="93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DO5" s="93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DP5" s="93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DQ5" s="93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DR5" s="93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:122" s="2" customFormat="1" ht="52.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>43</v>
-      </c>
       <c r="C6" s="90" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="91" t="s">
         <v>209</v>
       </c>
-      <c r="D6" s="91" t="s">
+      <c r="E6" s="91" t="s">
         <v>210</v>
       </c>
-      <c r="E6" s="91" t="s">
+      <c r="F6" s="91" t="s">
         <v>211</v>
       </c>
-      <c r="F6" s="91" t="s">
+      <c r="G6" s="91" t="s">
         <v>212</v>
       </c>
-      <c r="G6" s="91" t="s">
+      <c r="H6" s="91" t="s">
         <v>213</v>
       </c>
-      <c r="H6" s="91" t="s">
+      <c r="I6" s="91" t="s">
         <v>214</v>
       </c>
-      <c r="I6" s="91" t="s">
+      <c r="J6" s="91" t="s">
         <v>215</v>
       </c>
-      <c r="J6" s="91" t="s">
+      <c r="K6" s="91" t="s">
         <v>216</v>
       </c>
-      <c r="K6" s="91" t="s">
+      <c r="L6" s="91" t="s">
         <v>217</v>
       </c>
-      <c r="L6" s="91" t="s">
+      <c r="M6" s="91" t="s">
         <v>218</v>
       </c>
-      <c r="M6" s="91" t="s">
+      <c r="N6" s="91" t="s">
         <v>219</v>
       </c>
-      <c r="N6" s="91" t="s">
+      <c r="O6" s="91" t="s">
         <v>220</v>
       </c>
-      <c r="O6" s="91" t="s">
+      <c r="P6" s="91" t="s">
         <v>221</v>
       </c>
-      <c r="P6" s="91" t="s">
+      <c r="Q6" s="91" t="s">
         <v>222</v>
       </c>
-      <c r="Q6" s="91" t="s">
+      <c r="R6" s="91" t="s">
         <v>223</v>
       </c>
-      <c r="R6" s="91" t="s">
+      <c r="S6" s="91" t="s">
         <v>224</v>
       </c>
-      <c r="S6" s="91" t="s">
+      <c r="T6" s="91" t="s">
         <v>225</v>
       </c>
-      <c r="T6" s="91" t="s">
+      <c r="U6" s="91" t="s">
+        <v>326</v>
+      </c>
+      <c r="V6" s="91" t="s">
+        <v>225</v>
+      </c>
+      <c r="W6" s="91" t="s">
         <v>226</v>
-      </c>
-      <c r="U6" s="91" t="s">
-        <v>328</v>
-      </c>
-      <c r="V6" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="W6" s="91" t="s">
-        <v>227</v>
       </c>
       <c r="X6" s="91"/>
       <c r="Y6" s="91" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z6" s="91" t="s">
         <v>228</v>
       </c>
-      <c r="Z6" s="91" t="s">
+      <c r="AA6" s="91" t="s">
         <v>229</v>
       </c>
-      <c r="AA6" s="91" t="s">
+      <c r="AB6" s="91" t="s">
         <v>230</v>
       </c>
-      <c r="AB6" s="91" t="s">
+      <c r="AC6" s="91" t="s">
         <v>231</v>
       </c>
-      <c r="AC6" s="91" t="s">
+      <c r="AD6" s="91" t="s">
         <v>232</v>
       </c>
-      <c r="AD6" s="91" t="s">
+      <c r="AE6" s="91" t="s">
         <v>233</v>
       </c>
-      <c r="AE6" s="91" t="s">
+      <c r="AF6" s="91" t="s">
         <v>234</v>
       </c>
-      <c r="AF6" s="91" t="s">
+      <c r="AG6" s="91" t="s">
         <v>235</v>
       </c>
-      <c r="AG6" s="91" t="s">
+      <c r="AH6" s="91" t="s">
         <v>236</v>
       </c>
-      <c r="AH6" s="91" t="s">
+      <c r="AI6" s="91" t="s">
         <v>237</v>
       </c>
-      <c r="AI6" s="91" t="s">
+      <c r="AJ6" s="91" t="s">
         <v>238</v>
       </c>
-      <c r="AJ6" s="91" t="s">
+      <c r="AK6" s="91" t="s">
         <v>239</v>
       </c>
-      <c r="AK6" s="91" t="s">
+      <c r="AL6" s="91" t="s">
         <v>240</v>
       </c>
-      <c r="AL6" s="91" t="s">
+      <c r="AM6" s="91" t="s">
+        <v>327</v>
+      </c>
+      <c r="AN6" s="91" t="s">
         <v>241</v>
       </c>
-      <c r="AM6" s="91" t="s">
+      <c r="AO6" s="91" t="s">
+        <v>242</v>
+      </c>
+      <c r="AP6" s="91" t="s">
+        <v>243</v>
+      </c>
+      <c r="AQ6" s="91" t="s">
+        <v>244</v>
+      </c>
+      <c r="AR6" s="91" t="s">
+        <v>245</v>
+      </c>
+      <c r="AS6" s="91" t="s">
+        <v>246</v>
+      </c>
+      <c r="AT6" s="91" t="s">
+        <v>247</v>
+      </c>
+      <c r="AU6" s="91" t="s">
+        <v>248</v>
+      </c>
+      <c r="AV6" s="91" t="s">
+        <v>249</v>
+      </c>
+      <c r="AW6" s="91" t="s">
+        <v>250</v>
+      </c>
+      <c r="AX6" s="91" t="s">
+        <v>251</v>
+      </c>
+      <c r="AY6" s="91" t="s">
+        <v>252</v>
+      </c>
+      <c r="AZ6" s="91" t="s">
+        <v>253</v>
+      </c>
+      <c r="BA6" s="91" t="s">
+        <v>254</v>
+      </c>
+      <c r="BB6" s="91" t="s">
+        <v>255</v>
+      </c>
+      <c r="BC6" s="91" t="s">
+        <v>256</v>
+      </c>
+      <c r="BD6" s="91" t="s">
+        <v>257</v>
+      </c>
+      <c r="BE6" s="91" t="s">
+        <v>258</v>
+      </c>
+      <c r="BF6" s="91" t="s">
+        <v>259</v>
+      </c>
+      <c r="BG6" s="91" t="s">
+        <v>260</v>
+      </c>
+      <c r="BH6" s="91" t="s">
+        <v>261</v>
+      </c>
+      <c r="BI6" s="91" t="s">
+        <v>262</v>
+      </c>
+      <c r="BJ6" s="91" t="s">
+        <v>263</v>
+      </c>
+      <c r="BK6" s="91" t="s">
+        <v>264</v>
+      </c>
+      <c r="BL6" s="91" t="s">
+        <v>265</v>
+      </c>
+      <c r="BM6" s="91" t="s">
+        <v>266</v>
+      </c>
+      <c r="BN6" s="91" t="s">
+        <v>328</v>
+      </c>
+      <c r="BO6" s="91" t="s">
         <v>329</v>
       </c>
-      <c r="AN6" s="91" t="s">
-        <v>242</v>
-      </c>
-      <c r="AO6" s="91" t="s">
-        <v>243</v>
-      </c>
-      <c r="AP6" s="91" t="s">
-        <v>244</v>
-      </c>
-      <c r="AQ6" s="91" t="s">
-        <v>245</v>
-      </c>
-      <c r="AR6" s="91" t="s">
-        <v>246</v>
-      </c>
-      <c r="AS6" s="91" t="s">
-        <v>247</v>
-      </c>
-      <c r="AT6" s="91" t="s">
-        <v>248</v>
-      </c>
-      <c r="AU6" s="91" t="s">
-        <v>249</v>
-      </c>
-      <c r="AV6" s="91" t="s">
-        <v>250</v>
-      </c>
-      <c r="AW6" s="91" t="s">
-        <v>251</v>
-      </c>
-      <c r="AX6" s="91" t="s">
-        <v>252</v>
-      </c>
-      <c r="AY6" s="91" t="s">
-        <v>253</v>
-      </c>
-      <c r="AZ6" s="91" t="s">
-        <v>254</v>
-      </c>
-      <c r="BA6" s="91" t="s">
-        <v>255</v>
-      </c>
-      <c r="BB6" s="91" t="s">
-        <v>256</v>
-      </c>
-      <c r="BC6" s="91" t="s">
-        <v>257</v>
-      </c>
-      <c r="BD6" s="91" t="s">
-        <v>258</v>
-      </c>
-      <c r="BE6" s="91" t="s">
-        <v>259</v>
-      </c>
-      <c r="BF6" s="91" t="s">
-        <v>260</v>
-      </c>
-      <c r="BG6" s="91" t="s">
-        <v>261</v>
-      </c>
-      <c r="BH6" s="91" t="s">
-        <v>262</v>
-      </c>
-      <c r="BI6" s="91" t="s">
-        <v>263</v>
-      </c>
-      <c r="BJ6" s="91" t="s">
-        <v>264</v>
-      </c>
-      <c r="BK6" s="91" t="s">
-        <v>265</v>
-      </c>
-      <c r="BL6" s="91" t="s">
-        <v>266</v>
-      </c>
-      <c r="BM6" s="91" t="s">
+      <c r="BP6" s="91" t="s">
+        <v>330</v>
+      </c>
+      <c r="BQ6" s="91" t="s">
+        <v>331</v>
+      </c>
+      <c r="BR6" s="91" t="s">
+        <v>332</v>
+      </c>
+      <c r="BS6" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="BN6" s="91" t="s">
-        <v>330</v>
-      </c>
-      <c r="BO6" s="91" t="s">
+      <c r="BT6" s="91" t="s">
+        <v>268</v>
+      </c>
+      <c r="BU6" s="91" t="s">
+        <v>269</v>
+      </c>
+      <c r="BV6" s="91" t="s">
+        <v>333</v>
+      </c>
+      <c r="BW6" s="91" t="s">
+        <v>334</v>
+      </c>
+      <c r="BX6" s="91" t="s">
+        <v>270</v>
+      </c>
+      <c r="BY6" s="91" t="s">
+        <v>332</v>
+      </c>
+      <c r="BZ6" s="91" t="s">
+        <v>271</v>
+      </c>
+      <c r="CA6" s="91" t="s">
+        <v>272</v>
+      </c>
+      <c r="CB6" s="91" t="s">
+        <v>273</v>
+      </c>
+      <c r="CC6" s="91" t="s">
+        <v>274</v>
+      </c>
+      <c r="CD6" s="91" t="s">
+        <v>275</v>
+      </c>
+      <c r="CE6" s="91" t="s">
+        <v>276</v>
+      </c>
+      <c r="CF6" s="91" t="s">
+        <v>277</v>
+      </c>
+      <c r="CG6" s="91" t="s">
         <v>331</v>
       </c>
-      <c r="BP6" s="91" t="s">
-        <v>332</v>
-      </c>
-      <c r="BQ6" s="91" t="s">
-        <v>333</v>
-      </c>
-      <c r="BR6" s="91" t="s">
-        <v>334</v>
-      </c>
-      <c r="BS6" s="91" t="s">
-        <v>268</v>
-      </c>
-      <c r="BT6" s="91" t="s">
-        <v>269</v>
-      </c>
-      <c r="BU6" s="91" t="s">
-        <v>270</v>
-      </c>
-      <c r="BV6" s="91" t="s">
+      <c r="CH6" s="91" t="s">
+        <v>278</v>
+      </c>
+      <c r="CI6" s="91" t="s">
+        <v>279</v>
+      </c>
+      <c r="CJ6" s="91" t="s">
+        <v>280</v>
+      </c>
+      <c r="CK6" s="91" t="s">
+        <v>281</v>
+      </c>
+      <c r="CL6" s="91" t="s">
+        <v>282</v>
+      </c>
+      <c r="CM6" s="91" t="s">
+        <v>283</v>
+      </c>
+      <c r="CN6" s="91" t="s">
+        <v>284</v>
+      </c>
+      <c r="CO6" s="91" t="s">
+        <v>285</v>
+      </c>
+      <c r="CP6" s="91" t="s">
+        <v>286</v>
+      </c>
+      <c r="CQ6" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="CR6" s="91" t="s">
+        <v>288</v>
+      </c>
+      <c r="CS6" s="91" t="s">
         <v>335</v>
       </c>
-      <c r="BW6" s="91" t="s">
-        <v>336</v>
-      </c>
-      <c r="BX6" s="91" t="s">
-        <v>271</v>
-      </c>
-      <c r="BY6" s="91" t="s">
-        <v>334</v>
-      </c>
-      <c r="BZ6" s="91" t="s">
-        <v>272</v>
-      </c>
-      <c r="CA6" s="91" t="s">
-        <v>273</v>
-      </c>
-      <c r="CB6" s="91" t="s">
-        <v>274</v>
-      </c>
-      <c r="CC6" s="91" t="s">
-        <v>275</v>
-      </c>
-      <c r="CD6" s="91" t="s">
-        <v>276</v>
-      </c>
-      <c r="CE6" s="91" t="s">
-        <v>277</v>
-      </c>
-      <c r="CF6" s="91" t="s">
-        <v>278</v>
-      </c>
-      <c r="CG6" s="91" t="s">
-        <v>333</v>
-      </c>
-      <c r="CH6" s="91" t="s">
-        <v>279</v>
-      </c>
-      <c r="CI6" s="91" t="s">
-        <v>280</v>
-      </c>
-      <c r="CJ6" s="91" t="s">
-        <v>281</v>
-      </c>
-      <c r="CK6" s="91" t="s">
-        <v>282</v>
-      </c>
-      <c r="CL6" s="91" t="s">
-        <v>283</v>
-      </c>
-      <c r="CM6" s="91" t="s">
-        <v>284</v>
-      </c>
-      <c r="CN6" s="91" t="s">
-        <v>285</v>
-      </c>
-      <c r="CO6" s="91" t="s">
-        <v>286</v>
-      </c>
-      <c r="CP6" s="91" t="s">
-        <v>287</v>
-      </c>
-      <c r="CQ6" s="91" t="s">
-        <v>288</v>
-      </c>
-      <c r="CR6" s="91" t="s">
+      <c r="CT6" s="91" t="s">
         <v>289</v>
       </c>
-      <c r="CS6" s="91" t="s">
-        <v>337</v>
-      </c>
-      <c r="CT6" s="91" t="s">
+      <c r="CU6" s="91" t="s">
         <v>290</v>
       </c>
-      <c r="CU6" s="91" t="s">
+      <c r="CV6" s="91" t="s">
         <v>291</v>
       </c>
-      <c r="CV6" s="91" t="s">
+      <c r="CW6" s="91" t="s">
         <v>292</v>
       </c>
-      <c r="CW6" s="91" t="s">
+      <c r="CX6" s="91" t="s">
         <v>293</v>
       </c>
-      <c r="CX6" s="91" t="s">
+      <c r="CY6" s="91" t="s">
         <v>294</v>
       </c>
-      <c r="CY6" s="91" t="s">
+      <c r="CZ6" s="91" t="s">
         <v>295</v>
       </c>
-      <c r="CZ6" s="91" t="s">
+      <c r="DA6" s="91" t="s">
         <v>296</v>
       </c>
-      <c r="DA6" s="91" t="s">
+      <c r="DB6" s="91" t="s">
         <v>297</v>
       </c>
-      <c r="DB6" s="91" t="s">
+      <c r="DC6" s="91" t="s">
         <v>298</v>
       </c>
-      <c r="DC6" s="91" t="s">
+      <c r="DD6" s="91" t="s">
         <v>299</v>
-      </c>
-      <c r="DD6" s="91" t="s">
-        <v>300</v>
       </c>
       <c r="DE6" s="92"/>
       <c r="DF6" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="DG6" s="92" t="s">
         <v>301</v>
       </c>
-      <c r="DG6" s="92" t="s">
+      <c r="DH6" s="92" t="s">
         <v>302</v>
       </c>
-      <c r="DH6" s="92" t="s">
+      <c r="DI6" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="DJ6" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="DK6" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="DL6" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="DM6" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="DN6" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="DO6" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="DP6" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="DQ6" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="DR6" s="92" t="s">
         <v>303</v>
       </c>
-      <c r="DI6" s="92" t="s">
-        <v>303</v>
-      </c>
-      <c r="DJ6" s="92" t="s">
-        <v>303</v>
-      </c>
-      <c r="DK6" s="92" t="s">
-        <v>303</v>
-      </c>
-      <c r="DL6" s="92" t="s">
-        <v>303</v>
-      </c>
-      <c r="DM6" s="92" t="s">
-        <v>303</v>
-      </c>
-      <c r="DN6" s="92" t="s">
-        <v>303</v>
-      </c>
-      <c r="DO6" s="92" t="s">
-        <v>303</v>
-      </c>
-      <c r="DP6" s="92" t="s">
-        <v>303</v>
-      </c>
-      <c r="DQ6" s="92" t="s">
-        <v>303</v>
-      </c>
-      <c r="DR6" s="92" t="s">
-        <v>304</v>
-      </c>
     </row>
     <row r="7" spans="1:122" x14ac:dyDescent="0.3">
-      <c r="A7" s="108"/>
+      <c r="A7" s="112"/>
       <c r="B7" s="5"/>
       <c r="C7" s="17"/>
       <c r="D7" s="18"/>
@@ -6532,8 +6571,8 @@
       <c r="CP7" s="19"/>
       <c r="CQ7" s="18"/>
       <c r="CR7" s="18"/>
-      <c r="CS7" s="110" t="s">
-        <v>338</v>
+      <c r="CS7" s="100" t="s">
+        <v>336</v>
       </c>
       <c r="CT7" s="18"/>
       <c r="CU7" s="18"/>
@@ -6562,7 +6601,7 @@
       <c r="DR7" s="20"/>
     </row>
     <row r="8" spans="1:122" x14ac:dyDescent="0.3">
-      <c r="A8" s="108"/>
+      <c r="A8" s="104"/>
       <c r="B8" s="5"/>
       <c r="C8" s="21"/>
       <c r="CJ8" s="95"/>
@@ -6577,7 +6616,7 @@
       <c r="DR8" s="22"/>
     </row>
     <row r="9" spans="1:122" x14ac:dyDescent="0.3">
-      <c r="A9" s="108"/>
+      <c r="A9" s="104"/>
       <c r="B9" s="5"/>
       <c r="C9" s="21"/>
       <c r="CJ9" s="95"/>
@@ -6592,7 +6631,7 @@
       <c r="DR9" s="22"/>
     </row>
     <row r="10" spans="1:122" x14ac:dyDescent="0.3">
-      <c r="A10" s="108"/>
+      <c r="A10" s="104"/>
       <c r="B10" s="5"/>
       <c r="C10" s="21"/>
       <c r="CJ10" s="95"/>
@@ -6607,7 +6646,7 @@
       <c r="DR10" s="22"/>
     </row>
     <row r="11" spans="1:122" x14ac:dyDescent="0.3">
-      <c r="A11" s="108"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="5"/>
       <c r="C11" s="21"/>
       <c r="CJ11" s="95"/>
@@ -6622,7 +6661,7 @@
       <c r="DR11" s="22"/>
     </row>
     <row r="12" spans="1:122" x14ac:dyDescent="0.3">
-      <c r="A12" s="108"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="5"/>
       <c r="C12" s="21"/>
       <c r="CJ12" s="95"/>
@@ -6637,7 +6676,7 @@
       <c r="DR12" s="22"/>
     </row>
     <row r="13" spans="1:122" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="108"/>
+      <c r="A13" s="104"/>
       <c r="B13" s="5"/>
       <c r="C13" s="21"/>
       <c r="CJ13" s="95"/>
@@ -6652,7 +6691,7 @@
       <c r="DR13" s="22"/>
     </row>
     <row r="14" spans="1:122" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="108"/>
+      <c r="A14" s="104"/>
       <c r="B14" s="5"/>
       <c r="C14" s="21"/>
       <c r="CJ14" s="95"/>
@@ -6667,7 +6706,7 @@
       <c r="DR14" s="22"/>
     </row>
     <row r="15" spans="1:122" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="108"/>
+      <c r="A15" s="104"/>
       <c r="B15" s="5"/>
       <c r="C15" s="21"/>
       <c r="CJ15" s="95"/>
@@ -6682,7 +6721,7 @@
       <c r="DR15" s="22"/>
     </row>
     <row r="16" spans="1:122" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="109"/>
+      <c r="A16" s="105"/>
       <c r="B16" s="6"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
@@ -6810,48 +6849,48 @@
     <mergeCell ref="A7:A16"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="CT5" r:id="rId1" xr:uid="{72B74336-2CEF-41FE-9DEA-569F537AAC53}"/>
-    <hyperlink ref="DF5" r:id="rId2" xr:uid="{0BCBBCDA-D54E-473F-A6FF-214BAF7E0602}"/>
-    <hyperlink ref="DG5" r:id="rId3" xr:uid="{519370B5-9E22-4546-8E09-9C4141372EC4}"/>
-    <hyperlink ref="AF4" r:id="rId4" xr:uid="{E6789A15-5938-4B34-9060-B643446ED004}"/>
-    <hyperlink ref="AF5" r:id="rId5" xr:uid="{143B8C4A-4E44-4AE6-B837-6E60BB10B7CE}"/>
-    <hyperlink ref="AH4" r:id="rId6" xr:uid="{043D07EC-33CA-48F9-9214-0ED5BEB776CD}"/>
-    <hyperlink ref="C5" r:id="rId7" xr:uid="{BA2EAFA6-E280-495B-99DB-7CA2DFDD2D6F}"/>
-    <hyperlink ref="C4" r:id="rId8" xr:uid="{E0F912F5-B577-4CF6-A90E-B869B48A6758}"/>
-    <hyperlink ref="AM5" r:id="rId9" xr:uid="{77D1B38F-6E12-460C-814C-D226A6F04744}"/>
-    <hyperlink ref="AW4" r:id="rId10" xr:uid="{FE39A794-4E6C-4EFA-B975-47715C6672CA}"/>
-    <hyperlink ref="BC4" r:id="rId11" xr:uid="{8D2B0223-3851-40C0-9207-4F2EA0D184CE}"/>
-    <hyperlink ref="BD4" r:id="rId12" xr:uid="{437FB5A1-782A-4DF7-9967-45DA047AC799}"/>
-    <hyperlink ref="BB4" r:id="rId13" xr:uid="{13BC07A8-7C0A-4CB3-90E9-81D6D7915601}"/>
-    <hyperlink ref="BB5" r:id="rId14" xr:uid="{9F4AD485-3DA1-4285-98AF-775EA26CFBB7}"/>
-    <hyperlink ref="BK4" r:id="rId15" xr:uid="{FE5F9630-F8EB-41ED-B89B-646A36A3D724}"/>
-    <hyperlink ref="BL4" r:id="rId16" xr:uid="{F7FAFAEE-AFED-44BC-898A-4B28BECEEEC0}"/>
-    <hyperlink ref="BG4" r:id="rId17" xr:uid="{6392C557-33BF-4C21-B4B3-8370B9D1A803}"/>
-    <hyperlink ref="BG5" r:id="rId18" xr:uid="{3BB86668-5F76-4BD2-845B-2086A46A8366}"/>
-    <hyperlink ref="BK5" r:id="rId19" xr:uid="{CF78E667-0EBD-4C76-A0C3-AD4D3B9FCDFE}"/>
-    <hyperlink ref="BH4" r:id="rId20" xr:uid="{9525C054-830C-4B9B-8A41-FA4C8339288B}"/>
-    <hyperlink ref="BI4" r:id="rId21" xr:uid="{0558D85B-AFC1-46E5-8383-92416B1F79CC}"/>
-    <hyperlink ref="BJ4" r:id="rId22" xr:uid="{38B88F25-B4B7-48AD-9F47-346CC191001C}"/>
-    <hyperlink ref="BU5" r:id="rId23" xr:uid="{24266FE5-190B-408A-8E00-56323CBFA8C7}"/>
-    <hyperlink ref="BX5" r:id="rId24" xr:uid="{E577EE4F-07E4-4A25-B7F4-AB8BFB3E8BA5}"/>
-    <hyperlink ref="BZ5" r:id="rId25" xr:uid="{C4B4918D-7791-4DE2-82EB-C679628ECA9A}"/>
-    <hyperlink ref="BU4" r:id="rId26" xr:uid="{33FCFA13-BDC1-40E4-8BBC-C4516A566CA2}"/>
-    <hyperlink ref="CA4" r:id="rId27" xr:uid="{5A8E17AA-23F0-4EDB-AF76-B3C65E0DDCAB}"/>
-    <hyperlink ref="BS5" r:id="rId28" xr:uid="{09B9DCA6-D216-4E2E-B795-16A204FEEC72}"/>
-    <hyperlink ref="CA5" r:id="rId29" xr:uid="{B1A0E9BC-8ADC-459D-9D13-3635D6EE3D1D}"/>
-    <hyperlink ref="BZ4" r:id="rId30" xr:uid="{E97FB282-C0C0-46CC-9409-9FE42D427E89}"/>
-    <hyperlink ref="CB4" r:id="rId31" xr:uid="{39360677-EA55-4BBE-ABC7-EBEFFFCBD430}"/>
-    <hyperlink ref="BN5" r:id="rId32" xr:uid="{969FA93B-86B6-4814-BD1C-E78A60533950}"/>
-    <hyperlink ref="BO5" r:id="rId33" xr:uid="{CE078588-0D15-4B29-9D3A-40EC981605F3}"/>
-    <hyperlink ref="BO4" r:id="rId34" xr:uid="{EC8C4ACC-9A50-44B6-9A6F-A09D41227216}"/>
-    <hyperlink ref="BP5" r:id="rId35" xr:uid="{37A73806-E695-45FC-92CA-2280673B33BA}"/>
-    <hyperlink ref="BP4" r:id="rId36" xr:uid="{AD12C858-A6F8-461E-B119-33FC6D01F11A}"/>
-    <hyperlink ref="BV4" r:id="rId37" xr:uid="{90534F12-B95A-4AAD-AEDB-A256614DB0D6}"/>
-    <hyperlink ref="BV5" r:id="rId38" xr:uid="{C20BA0B6-7C2F-41CF-9683-8E8C6BA960B7}"/>
-    <hyperlink ref="CE4" r:id="rId39" xr:uid="{01F0DA22-AD76-44A4-9D99-DD5EAE634306}"/>
-    <hyperlink ref="CE5" r:id="rId40" xr:uid="{7FB6A789-D621-4988-B107-E8BAC64828F6}"/>
-    <hyperlink ref="CF4" r:id="rId41" xr:uid="{52C90264-B3A6-4214-873C-BB86D485CBFA}"/>
-    <hyperlink ref="CS5" r:id="rId42" xr:uid="{6592FA46-4216-41E6-9BFC-376DD403D7ED}"/>
+    <hyperlink ref="CS5" r:id="rId1" xr:uid="{6592FA46-4216-41E6-9BFC-376DD403D7ED}"/>
+    <hyperlink ref="CF4" r:id="rId2" xr:uid="{52C90264-B3A6-4214-873C-BB86D485CBFA}"/>
+    <hyperlink ref="CE5" r:id="rId3" xr:uid="{7FB6A789-D621-4988-B107-E8BAC64828F6}"/>
+    <hyperlink ref="CE4" r:id="rId4" xr:uid="{01F0DA22-AD76-44A4-9D99-DD5EAE634306}"/>
+    <hyperlink ref="BV5" r:id="rId5" xr:uid="{C20BA0B6-7C2F-41CF-9683-8E8C6BA960B7}"/>
+    <hyperlink ref="BV4" r:id="rId6" xr:uid="{90534F12-B95A-4AAD-AEDB-A256614DB0D6}"/>
+    <hyperlink ref="BP4" r:id="rId7" xr:uid="{AD12C858-A6F8-461E-B119-33FC6D01F11A}"/>
+    <hyperlink ref="BP5" r:id="rId8" xr:uid="{37A73806-E695-45FC-92CA-2280673B33BA}"/>
+    <hyperlink ref="BO4" r:id="rId9" xr:uid="{EC8C4ACC-9A50-44B6-9A6F-A09D41227216}"/>
+    <hyperlink ref="BO5" r:id="rId10" xr:uid="{CE078588-0D15-4B29-9D3A-40EC981605F3}"/>
+    <hyperlink ref="BN5" r:id="rId11" xr:uid="{969FA93B-86B6-4814-BD1C-E78A60533950}"/>
+    <hyperlink ref="CB4" r:id="rId12" xr:uid="{39360677-EA55-4BBE-ABC7-EBEFFFCBD430}"/>
+    <hyperlink ref="BZ4" r:id="rId13" xr:uid="{E97FB282-C0C0-46CC-9409-9FE42D427E89}"/>
+    <hyperlink ref="CA5" r:id="rId14" xr:uid="{B1A0E9BC-8ADC-459D-9D13-3635D6EE3D1D}"/>
+    <hyperlink ref="BS5" r:id="rId15" xr:uid="{09B9DCA6-D216-4E2E-B795-16A204FEEC72}"/>
+    <hyperlink ref="CA4" r:id="rId16" xr:uid="{5A8E17AA-23F0-4EDB-AF76-B3C65E0DDCAB}"/>
+    <hyperlink ref="BU4" r:id="rId17" xr:uid="{33FCFA13-BDC1-40E4-8BBC-C4516A566CA2}"/>
+    <hyperlink ref="BZ5" r:id="rId18" xr:uid="{C4B4918D-7791-4DE2-82EB-C679628ECA9A}"/>
+    <hyperlink ref="BX5" r:id="rId19" xr:uid="{E577EE4F-07E4-4A25-B7F4-AB8BFB3E8BA5}"/>
+    <hyperlink ref="BU5" r:id="rId20" xr:uid="{24266FE5-190B-408A-8E00-56323CBFA8C7}"/>
+    <hyperlink ref="BJ4" r:id="rId21" xr:uid="{38B88F25-B4B7-48AD-9F47-346CC191001C}"/>
+    <hyperlink ref="BI4" r:id="rId22" xr:uid="{0558D85B-AFC1-46E5-8383-92416B1F79CC}"/>
+    <hyperlink ref="BH4" r:id="rId23" xr:uid="{9525C054-830C-4B9B-8A41-FA4C8339288B}"/>
+    <hyperlink ref="BK5" r:id="rId24" xr:uid="{CF78E667-0EBD-4C76-A0C3-AD4D3B9FCDFE}"/>
+    <hyperlink ref="BG5" r:id="rId25" xr:uid="{3BB86668-5F76-4BD2-845B-2086A46A8366}"/>
+    <hyperlink ref="BG4" r:id="rId26" xr:uid="{6392C557-33BF-4C21-B4B3-8370B9D1A803}"/>
+    <hyperlink ref="BL4" r:id="rId27" xr:uid="{F7FAFAEE-AFED-44BC-898A-4B28BECEEEC0}"/>
+    <hyperlink ref="BK4" r:id="rId28" xr:uid="{FE5F9630-F8EB-41ED-B89B-646A36A3D724}"/>
+    <hyperlink ref="BB5" r:id="rId29" xr:uid="{9F4AD485-3DA1-4285-98AF-775EA26CFBB7}"/>
+    <hyperlink ref="BB4" r:id="rId30" xr:uid="{13BC07A8-7C0A-4CB3-90E9-81D6D7915601}"/>
+    <hyperlink ref="BD4" r:id="rId31" xr:uid="{437FB5A1-782A-4DF7-9967-45DA047AC799}"/>
+    <hyperlink ref="BC4" r:id="rId32" xr:uid="{8D2B0223-3851-40C0-9207-4F2EA0D184CE}"/>
+    <hyperlink ref="AW4" r:id="rId33" xr:uid="{FE39A794-4E6C-4EFA-B975-47715C6672CA}"/>
+    <hyperlink ref="AM5" r:id="rId34" xr:uid="{77D1B38F-6E12-460C-814C-D226A6F04744}"/>
+    <hyperlink ref="C4" r:id="rId35" xr:uid="{E0F912F5-B577-4CF6-A90E-B869B48A6758}"/>
+    <hyperlink ref="C5" r:id="rId36" xr:uid="{BA2EAFA6-E280-495B-99DB-7CA2DFDD2D6F}"/>
+    <hyperlink ref="AH4" r:id="rId37" xr:uid="{043D07EC-33CA-48F9-9214-0ED5BEB776CD}"/>
+    <hyperlink ref="AF5" r:id="rId38" xr:uid="{143B8C4A-4E44-4AE6-B837-6E60BB10B7CE}"/>
+    <hyperlink ref="AF4" r:id="rId39" xr:uid="{E6789A15-5938-4B34-9060-B643446ED004}"/>
+    <hyperlink ref="DG5" r:id="rId40" xr:uid="{519370B5-9E22-4546-8E09-9C4141372EC4}"/>
+    <hyperlink ref="DF5" r:id="rId41" xr:uid="{0BCBBCDA-D54E-473F-A6FF-214BAF7E0602}"/>
+    <hyperlink ref="CT5" r:id="rId42" xr:uid="{72B74336-2CEF-41FE-9DEA-569F537AAC53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rebarnding to "FHIRSheets" Preparing to move towards CDCgov
</commit_message>
<xml_diff>
--- a/src/resources/Fhir_Cohort_Import_Template.xlsx
+++ b/src/resources/Fhir_Cohort_Import_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\T21_Connectathon_Sets\Fhir_CohortPython_Generation\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E559D7E-615E-471A-9B13-B24F61D73FAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A11CBB-5D90-4F8F-A2F0-87344208EF32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8196" xr2:uid="{B7CAF98F-F4CF-4673-A736-BDE9BA8D985C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8196" firstSheet="1" activeTab="5" xr2:uid="{B7CAF98F-F4CF-4673-A736-BDE9BA8D985C}"/>
   </bookViews>
   <sheets>
     <sheet name="How To Use This Workbook" sheetId="6" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ResourceLinks" sheetId="3" r:id="rId3"/>
     <sheet name="PatientData" sheetId="1" r:id="rId4"/>
     <sheet name="ReferenceSheet" sheetId="5" r:id="rId5"/>
+    <sheet name="Drop Down Selections" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -110,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="395">
   <si>
     <t>How To Use This Workbook</t>
   </si>
@@ -1137,6 +1138,209 @@
   </si>
   <si>
     <t>35^mg</t>
+  </si>
+  <si>
+    <t>PrimaryEncounter</t>
+  </si>
+  <si>
+    <t>Encounter</t>
+  </si>
+  <si>
+    <t>PrimaryPatient</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>Mother</t>
+  </si>
+  <si>
+    <t>RelatedPerson</t>
+  </si>
+  <si>
+    <t>PulseOximetry</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>American Indian or Alaska Native</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Black or African American</t>
+  </si>
+  <si>
+    <t>Native Hawaiian or Other Pacific Islander</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino</t>
+  </si>
+  <si>
+    <t>Non Hispanic or Latino</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>fax</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>pager</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>sms</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Telecom System (Type)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(MultipleResources)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ContactPoint)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.system</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Telecom use </t>
+  </si>
+  <si>
+    <t>https://hl7.org/fhir/r4/valueset-contact-point-use.html</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>work</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>old</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>suspended</t>
+  </si>
+  <si>
+    <t>inactive</t>
+  </si>
+  <si>
+    <t>planned</t>
+  </si>
+  <si>
+    <t>arrived</t>
+  </si>
+  <si>
+    <t>triaged</t>
+  </si>
+  <si>
+    <t>in-progress</t>
+  </si>
+  <si>
+    <t>onleave</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>cancelled</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/v3-ActCode^AMB^ambulatory</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/v3-ActCode^EMER^emergency</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/v3-ActCode^FLD^field</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/v3-ActCode^HH^home health</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/v3-ActCode^IMP^inpatient encounter</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/v3-ActCode^ACUTE^inpatient acute</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/v3-ActCode^NONAC^inpatient non-acute</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/v3-ActCode^OBSENC^observation encounter</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/v3-ActCode^PRENC^pre-admission</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/v3-ActCode^SS^short stay</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/v3-ActCode^VR^virtual</t>
   </si>
 </sst>
 </file>
@@ -1724,7 +1928,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1956,14 +2160,32 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1971,26 +2193,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2403,7 +2676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC3792E-0A86-43B6-8F3D-128E7961060A}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2416,39 +2689,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="106"/>
+      <c r="B1" s="109"/>
     </row>
     <row r="2" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
     </row>
     <row r="3" spans="1:3" ht="103.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="101"/>
+      <c r="B3" s="108"/>
     </row>
     <row r="4" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="108" t="s">
+      <c r="A4" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="108"/>
-      <c r="C4" s="108"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="107"/>
     </row>
     <row r="5" spans="1:3" ht="40.799999999999997" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="103"/>
+      <c r="B5" s="105"/>
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="101" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="97" t="s">
@@ -2456,7 +2729,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="109" t="s">
+      <c r="A7" s="101" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="97" t="s">
@@ -2464,7 +2737,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="109" t="s">
+      <c r="A8" s="101" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="97" t="s">
@@ -2472,7 +2745,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="101" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="97" t="s">
@@ -2480,47 +2753,47 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="107"/>
-      <c r="C10" s="107"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="106"/>
     </row>
     <row r="11" spans="1:3" ht="37.200000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="108" t="s">
         <v>305</v>
       </c>
-      <c r="B11" s="101"/>
+      <c r="B11" s="108"/>
     </row>
     <row r="12" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="102" t="s">
+      <c r="A12" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="102"/>
+      <c r="B12" s="104"/>
     </row>
     <row r="13" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="102" t="s">
+      <c r="A13" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="102"/>
+      <c r="B13" s="104"/>
     </row>
     <row r="14" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="102" t="s">
+      <c r="A14" s="104" t="s">
         <v>308</v>
       </c>
-      <c r="B14" s="102"/>
+      <c r="B14" s="104"/>
     </row>
     <row r="15" spans="1:3" ht="34.799999999999997" x14ac:dyDescent="0.35">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="110"/>
-      <c r="C15" s="110" t="s">
+      <c r="B15" s="102"/>
+      <c r="C15" s="102" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="111" t="s">
+      <c r="A16" s="103" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="97" t="s">
@@ -2531,7 +2804,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="111" t="s">
+      <c r="A17" s="103" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="97" t="s">
@@ -2542,7 +2815,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="111" t="s">
+      <c r="A18" s="103" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="97" t="s">
@@ -2553,7 +2826,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="111" t="s">
+      <c r="A19" s="103" t="s">
         <v>145</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2591,7 +2864,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2624,14 +2897,36 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C3" s="7"/>
+      <c r="A3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>194</v>
+      </c>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C4" s="7"/>
+      <c r="A4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>189</v>
+      </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>345</v>
+      </c>
+      <c r="B5" t="s">
+        <v>346</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
@@ -2640,7 +2935,15 @@
       <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C7" s="7"/>
+      <c r="A7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C8" s="7"/>
@@ -3540,7 +3843,7 @@
       <c r="DW6" s="15"/>
     </row>
     <row r="7" spans="1:127" x14ac:dyDescent="0.3">
-      <c r="A7" s="104"/>
+      <c r="A7" s="110"/>
       <c r="B7" s="26"/>
       <c r="C7" s="17"/>
       <c r="D7" s="18"/>
@@ -3650,7 +3953,7 @@
       <c r="DD7" s="20"/>
     </row>
     <row r="8" spans="1:127" x14ac:dyDescent="0.3">
-      <c r="A8" s="104"/>
+      <c r="A8" s="110"/>
       <c r="B8" s="5"/>
       <c r="C8" s="21"/>
       <c r="D8" s="8"/>
@@ -3760,7 +4063,7 @@
       <c r="DD8" s="22"/>
     </row>
     <row r="9" spans="1:127" x14ac:dyDescent="0.3">
-      <c r="A9" s="104"/>
+      <c r="A9" s="110"/>
       <c r="B9" s="5"/>
       <c r="C9" s="21"/>
       <c r="D9" s="8"/>
@@ -3870,7 +4173,7 @@
       <c r="DD9" s="22"/>
     </row>
     <row r="10" spans="1:127" x14ac:dyDescent="0.3">
-      <c r="A10" s="104"/>
+      <c r="A10" s="110"/>
       <c r="B10" s="5"/>
       <c r="C10" s="21"/>
       <c r="D10" s="8"/>
@@ -3980,7 +4283,7 @@
       <c r="DD10" s="22"/>
     </row>
     <row r="11" spans="1:127" x14ac:dyDescent="0.3">
-      <c r="A11" s="104"/>
+      <c r="A11" s="110"/>
       <c r="B11" s="5"/>
       <c r="C11" s="21"/>
       <c r="D11" s="8"/>
@@ -4090,7 +4393,7 @@
       <c r="DD11" s="22"/>
     </row>
     <row r="12" spans="1:127" x14ac:dyDescent="0.3">
-      <c r="A12" s="104"/>
+      <c r="A12" s="110"/>
       <c r="B12" s="5"/>
       <c r="C12" s="21"/>
       <c r="D12" s="8"/>
@@ -4200,7 +4503,7 @@
       <c r="DD12" s="22"/>
     </row>
     <row r="13" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="104"/>
+      <c r="A13" s="110"/>
       <c r="B13" s="5"/>
       <c r="C13" s="21"/>
       <c r="D13" s="8"/>
@@ -4310,7 +4613,7 @@
       <c r="DD13" s="22"/>
     </row>
     <row r="14" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="104"/>
+      <c r="A14" s="110"/>
       <c r="B14" s="5"/>
       <c r="C14" s="21"/>
       <c r="D14" s="8"/>
@@ -4420,7 +4723,7 @@
       <c r="DD14" s="22"/>
     </row>
     <row r="15" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="104"/>
+      <c r="A15" s="110"/>
       <c r="B15" s="5"/>
       <c r="C15" s="21"/>
       <c r="D15" s="8"/>
@@ -4530,7 +4833,7 @@
       <c r="DD15" s="22"/>
     </row>
     <row r="16" spans="1:127" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="105"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="6"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
@@ -4653,7 +4956,7 @@
   <dimension ref="A1:DR16"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -6601,7 +6904,7 @@
       <c r="DR7" s="20"/>
     </row>
     <row r="8" spans="1:122" x14ac:dyDescent="0.3">
-      <c r="A8" s="104"/>
+      <c r="A8" s="110"/>
       <c r="B8" s="5"/>
       <c r="C8" s="21"/>
       <c r="CJ8" s="95"/>
@@ -6616,7 +6919,7 @@
       <c r="DR8" s="22"/>
     </row>
     <row r="9" spans="1:122" x14ac:dyDescent="0.3">
-      <c r="A9" s="104"/>
+      <c r="A9" s="110"/>
       <c r="B9" s="5"/>
       <c r="C9" s="21"/>
       <c r="CJ9" s="95"/>
@@ -6631,7 +6934,7 @@
       <c r="DR9" s="22"/>
     </row>
     <row r="10" spans="1:122" x14ac:dyDescent="0.3">
-      <c r="A10" s="104"/>
+      <c r="A10" s="110"/>
       <c r="B10" s="5"/>
       <c r="C10" s="21"/>
       <c r="CJ10" s="95"/>
@@ -6646,7 +6949,7 @@
       <c r="DR10" s="22"/>
     </row>
     <row r="11" spans="1:122" x14ac:dyDescent="0.3">
-      <c r="A11" s="104"/>
+      <c r="A11" s="110"/>
       <c r="B11" s="5"/>
       <c r="C11" s="21"/>
       <c r="CJ11" s="95"/>
@@ -6661,7 +6964,7 @@
       <c r="DR11" s="22"/>
     </row>
     <row r="12" spans="1:122" x14ac:dyDescent="0.3">
-      <c r="A12" s="104"/>
+      <c r="A12" s="110"/>
       <c r="B12" s="5"/>
       <c r="C12" s="21"/>
       <c r="CJ12" s="95"/>
@@ -6676,7 +6979,7 @@
       <c r="DR12" s="22"/>
     </row>
     <row r="13" spans="1:122" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="104"/>
+      <c r="A13" s="110"/>
       <c r="B13" s="5"/>
       <c r="C13" s="21"/>
       <c r="CJ13" s="95"/>
@@ -6691,7 +6994,7 @@
       <c r="DR13" s="22"/>
     </row>
     <row r="14" spans="1:122" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="104"/>
+      <c r="A14" s="110"/>
       <c r="B14" s="5"/>
       <c r="C14" s="21"/>
       <c r="CJ14" s="95"/>
@@ -6706,7 +7009,7 @@
       <c r="DR14" s="22"/>
     </row>
     <row r="15" spans="1:122" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="104"/>
+      <c r="A15" s="110"/>
       <c r="B15" s="5"/>
       <c r="C15" s="21"/>
       <c r="CJ15" s="95"/>
@@ -6721,7 +7024,7 @@
       <c r="DR15" s="22"/>
     </row>
     <row r="16" spans="1:122" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="105"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="6"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
@@ -6894,4 +7197,1671 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2908121E-D5C1-4307-B451-FAE780135275}">
+  <dimension ref="A1:CF16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="30" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="116.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="56" width="30" style="2"/>
+    <col min="57" max="57" width="43" style="2" customWidth="1"/>
+    <col min="58" max="58" width="30" style="2"/>
+    <col min="59" max="59" width="43.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="60" max="16384" width="30" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:84" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="89" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>366</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="48" t="s">
+        <v>314</v>
+      </c>
+      <c r="L1" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="N1" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q1" s="50" t="s">
+        <v>315</v>
+      </c>
+      <c r="R1" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="S1" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="T1" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="U1" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="V1" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="W1" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="X1" s="52" t="s">
+        <v>317</v>
+      </c>
+      <c r="Y1" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z1" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA1" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB1" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC1" s="56" t="s">
+        <v>318</v>
+      </c>
+      <c r="AD1" s="56" t="s">
+        <v>319</v>
+      </c>
+      <c r="AE1" s="56" t="s">
+        <v>320</v>
+      </c>
+      <c r="AF1" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG1" s="56" t="s">
+        <v>321</v>
+      </c>
+      <c r="AH1" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="AI1" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ1" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK1" s="58" t="s">
+        <v>320</v>
+      </c>
+      <c r="AL1" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM1" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="AN1" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO1" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP1" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ1" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="AR1" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="AS1" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="AT1" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="AU1" s="62" t="s">
+        <v>323</v>
+      </c>
+      <c r="AV1" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW1" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX1" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="AY1" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="AZ1" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="BA1" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB1" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC1" s="66" t="s">
+        <v>122</v>
+      </c>
+      <c r="BD1" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="BE1" s="66" t="s">
+        <v>124</v>
+      </c>
+      <c r="BF1" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="BG1" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="BH1" s="68" t="s">
+        <v>107</v>
+      </c>
+      <c r="BI1" s="68" t="s">
+        <v>107</v>
+      </c>
+      <c r="BJ1" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="BK1" s="70" t="s">
+        <v>127</v>
+      </c>
+      <c r="BL1" s="70" t="s">
+        <v>128</v>
+      </c>
+      <c r="BM1" s="70" t="s">
+        <v>129</v>
+      </c>
+      <c r="BN1" s="70" t="s">
+        <v>130</v>
+      </c>
+      <c r="BO1" s="70" t="s">
+        <v>131</v>
+      </c>
+      <c r="BP1" s="70" t="s">
+        <v>132</v>
+      </c>
+      <c r="BQ1" s="70" t="s">
+        <v>133</v>
+      </c>
+      <c r="BR1" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="BS1" s="70" t="s">
+        <v>135</v>
+      </c>
+      <c r="BT1" s="93" t="s">
+        <v>105</v>
+      </c>
+      <c r="BU1" s="93" t="s">
+        <v>136</v>
+      </c>
+      <c r="BV1" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="BW1" s="93" t="s">
+        <v>100</v>
+      </c>
+      <c r="BX1" s="93" t="s">
+        <v>108</v>
+      </c>
+      <c r="BY1" s="93" t="s">
+        <v>109</v>
+      </c>
+      <c r="BZ1" s="93" t="s">
+        <v>110</v>
+      </c>
+      <c r="CA1" s="93" t="s">
+        <v>111</v>
+      </c>
+      <c r="CB1" s="93" t="s">
+        <v>112</v>
+      </c>
+      <c r="CC1" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="CD1" s="93" t="s">
+        <v>114</v>
+      </c>
+      <c r="CE1" s="93" t="s">
+        <v>115</v>
+      </c>
+      <c r="CF1" s="93" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:84" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="113" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="89"/>
+      <c r="D2" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="J2" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="M2" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="N2" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q2" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="T2" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="U2" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z2" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA2" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB2" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC2" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD2" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE2" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF2" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG2" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH2" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI2" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="AJ2" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK2" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL2" s="58" t="s">
+        <v>144</v>
+      </c>
+      <c r="AM2" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN2" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO2" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="AP2" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ2" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="AR2" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="AS2" s="62" t="s">
+        <v>137</v>
+      </c>
+      <c r="AT2" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU2" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV2" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="AW2" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="AX2" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY2" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ2" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA2" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB2" s="64" t="s">
+        <v>151</v>
+      </c>
+      <c r="BC2" s="66" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD2" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="BE2" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="BF2" s="66" t="s">
+        <v>138</v>
+      </c>
+      <c r="BG2" s="68" t="s">
+        <v>137</v>
+      </c>
+      <c r="BH2" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="BI2" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="BJ2" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="BK2" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="BL2" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="BM2" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="BN2" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="BO2" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="BP2" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="BQ2" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="BR2" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="BS2" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="BT2" s="93" t="s">
+        <v>16</v>
+      </c>
+      <c r="BU2" s="93" t="s">
+        <v>142</v>
+      </c>
+      <c r="BV2" s="93" t="s">
+        <v>145</v>
+      </c>
+      <c r="BW2" s="93" t="s">
+        <v>16</v>
+      </c>
+      <c r="BX2" s="93" t="s">
+        <v>138</v>
+      </c>
+      <c r="BY2" s="93" t="s">
+        <v>141</v>
+      </c>
+      <c r="BZ2" s="93" t="s">
+        <v>146</v>
+      </c>
+      <c r="CA2" s="93" t="s">
+        <v>147</v>
+      </c>
+      <c r="CB2" s="93" t="s">
+        <v>148</v>
+      </c>
+      <c r="CC2" s="93" t="s">
+        <v>149</v>
+      </c>
+      <c r="CD2" s="93" t="s">
+        <v>142</v>
+      </c>
+      <c r="CE2" s="93" t="s">
+        <v>150</v>
+      </c>
+      <c r="CF2" s="93" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:84" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="114" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="94" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>368</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="I3" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="J3" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="K3" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="O3" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="P3" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q3" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="R3" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="S3" s="51"/>
+      <c r="T3" s="51"/>
+      <c r="U3" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="V3" s="53" t="s">
+        <v>171</v>
+      </c>
+      <c r="W3" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="X3" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y3" s="55" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z3" s="55" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA3" s="55"/>
+      <c r="AB3" s="57"/>
+      <c r="AC3" s="57" t="s">
+        <v>181</v>
+      </c>
+      <c r="AD3" s="57" t="s">
+        <v>181</v>
+      </c>
+      <c r="AE3" s="57" t="s">
+        <v>325</v>
+      </c>
+      <c r="AF3" s="57"/>
+      <c r="AG3" s="57"/>
+      <c r="AH3" s="57"/>
+      <c r="AI3" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ3" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="AK3" s="59" t="s">
+        <v>325</v>
+      </c>
+      <c r="AL3" s="59"/>
+      <c r="AM3" s="59"/>
+      <c r="AN3" s="59" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO3" s="61" t="s">
+        <v>178</v>
+      </c>
+      <c r="AP3" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="AQ3" s="61"/>
+      <c r="AR3" s="61"/>
+      <c r="AS3" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="AT3" s="63" t="s">
+        <v>181</v>
+      </c>
+      <c r="AU3" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="AV3" s="62"/>
+      <c r="AW3" s="62"/>
+      <c r="AX3" s="65" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY3" s="65" t="s">
+        <v>183</v>
+      </c>
+      <c r="AZ3" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="BA3" s="65"/>
+      <c r="BB3" s="65"/>
+      <c r="BC3" s="67" t="s">
+        <v>185</v>
+      </c>
+      <c r="BD3" s="67" t="s">
+        <v>186</v>
+      </c>
+      <c r="BE3" s="66"/>
+      <c r="BF3" s="66"/>
+      <c r="BG3" s="69"/>
+      <c r="BH3" s="69"/>
+      <c r="BI3" s="69"/>
+      <c r="BJ3" s="69"/>
+      <c r="BK3" s="71"/>
+      <c r="BL3" s="71"/>
+      <c r="BM3" s="71"/>
+      <c r="BN3" s="71"/>
+      <c r="BO3" s="71"/>
+      <c r="BP3" s="71"/>
+      <c r="BQ3" s="71"/>
+      <c r="BR3" s="71"/>
+      <c r="BS3" s="71" t="s">
+        <v>187</v>
+      </c>
+      <c r="BT3" s="93" t="s">
+        <v>188</v>
+      </c>
+      <c r="BU3" s="93"/>
+      <c r="BV3" s="93"/>
+      <c r="BW3" s="93"/>
+      <c r="BX3" s="93"/>
+      <c r="BY3" s="93"/>
+      <c r="BZ3" s="93"/>
+      <c r="CA3" s="93"/>
+      <c r="CB3" s="93"/>
+      <c r="CC3" s="93"/>
+      <c r="CD3" s="93"/>
+      <c r="CE3" s="93"/>
+      <c r="CF3" s="93"/>
+    </row>
+    <row r="4" spans="1:84" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="115" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="94" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="I4" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="J4" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="K4" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="L4" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="M4" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="N4" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="O4" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="P4" s="51" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q4" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="R4" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="S4" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="T4" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="U4" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="V4" s="52" t="s">
+        <v>196</v>
+      </c>
+      <c r="W4" s="52" t="s">
+        <v>196</v>
+      </c>
+      <c r="X4" s="52"/>
+      <c r="Y4" s="55" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z4" s="54" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA4" s="54" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB4" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC4" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="AD4" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="AE4" s="57" t="s">
+        <v>201</v>
+      </c>
+      <c r="AF4" s="57" t="s">
+        <v>201</v>
+      </c>
+      <c r="AG4" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="AH4" s="56" t="s">
+        <v>198</v>
+      </c>
+      <c r="AI4" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="AJ4" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="AK4" s="58" t="s">
+        <v>201</v>
+      </c>
+      <c r="AL4" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="AM4" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="AN4" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO4" s="61" t="s">
+        <v>200</v>
+      </c>
+      <c r="AP4" s="60" t="s">
+        <v>200</v>
+      </c>
+      <c r="AQ4" s="60" t="s">
+        <v>200</v>
+      </c>
+      <c r="AR4" s="61" t="s">
+        <v>200</v>
+      </c>
+      <c r="AS4" s="63" t="s">
+        <v>201</v>
+      </c>
+      <c r="AT4" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="AU4" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="AV4" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="AW4" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="AX4" s="64" t="s">
+        <v>202</v>
+      </c>
+      <c r="AY4" s="64" t="s">
+        <v>202</v>
+      </c>
+      <c r="AZ4" s="64" t="s">
+        <v>202</v>
+      </c>
+      <c r="BA4" s="64" t="s">
+        <v>202</v>
+      </c>
+      <c r="BB4" s="64"/>
+      <c r="BC4" s="66" t="s">
+        <v>203</v>
+      </c>
+      <c r="BD4" s="66" t="s">
+        <v>203</v>
+      </c>
+      <c r="BE4" s="66" t="s">
+        <v>203</v>
+      </c>
+      <c r="BF4" s="66" t="s">
+        <v>203</v>
+      </c>
+      <c r="BG4" s="69" t="s">
+        <v>204</v>
+      </c>
+      <c r="BH4" s="69" t="s">
+        <v>204</v>
+      </c>
+      <c r="BI4" s="68" t="s">
+        <v>204</v>
+      </c>
+      <c r="BJ4" s="68" t="s">
+        <v>205</v>
+      </c>
+      <c r="BK4" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="BL4" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="BM4" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="BN4" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="BO4" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="BP4" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="BQ4" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="BR4" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="BS4" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="BT4" s="93" t="s">
+        <v>207</v>
+      </c>
+      <c r="BU4" s="93" t="s">
+        <v>207</v>
+      </c>
+      <c r="BV4" s="93" t="s">
+        <v>201</v>
+      </c>
+      <c r="BW4" s="93" t="s">
+        <v>201</v>
+      </c>
+      <c r="BX4" s="93" t="s">
+        <v>201</v>
+      </c>
+      <c r="BY4" s="93" t="s">
+        <v>201</v>
+      </c>
+      <c r="BZ4" s="93" t="s">
+        <v>201</v>
+      </c>
+      <c r="CA4" s="93" t="s">
+        <v>201</v>
+      </c>
+      <c r="CB4" s="93" t="s">
+        <v>201</v>
+      </c>
+      <c r="CC4" s="93" t="s">
+        <v>201</v>
+      </c>
+      <c r="CD4" s="93" t="s">
+        <v>201</v>
+      </c>
+      <c r="CE4" s="93" t="s">
+        <v>201</v>
+      </c>
+      <c r="CF4" s="93" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:84" ht="52.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="90" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="91" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" s="91" t="s">
+        <v>210</v>
+      </c>
+      <c r="F5" s="91" t="s">
+        <v>365</v>
+      </c>
+      <c r="G5" s="91" t="s">
+        <v>367</v>
+      </c>
+      <c r="H5" s="91" t="s">
+        <v>234</v>
+      </c>
+      <c r="I5" s="91" t="s">
+        <v>248</v>
+      </c>
+      <c r="J5" s="91" t="s">
+        <v>249</v>
+      </c>
+      <c r="K5" s="91" t="s">
+        <v>250</v>
+      </c>
+      <c r="L5" s="91" t="s">
+        <v>251</v>
+      </c>
+      <c r="M5" s="91" t="s">
+        <v>252</v>
+      </c>
+      <c r="N5" s="91" t="s">
+        <v>253</v>
+      </c>
+      <c r="O5" s="91" t="s">
+        <v>254</v>
+      </c>
+      <c r="P5" s="91" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q5" s="91" t="s">
+        <v>256</v>
+      </c>
+      <c r="R5" s="91" t="s">
+        <v>257</v>
+      </c>
+      <c r="S5" s="91" t="s">
+        <v>258</v>
+      </c>
+      <c r="T5" s="91" t="s">
+        <v>259</v>
+      </c>
+      <c r="U5" s="91" t="s">
+        <v>260</v>
+      </c>
+      <c r="V5" s="91" t="s">
+        <v>261</v>
+      </c>
+      <c r="W5" s="91" t="s">
+        <v>262</v>
+      </c>
+      <c r="X5" s="91" t="s">
+        <v>263</v>
+      </c>
+      <c r="Y5" s="91" t="s">
+        <v>264</v>
+      </c>
+      <c r="Z5" s="91" t="s">
+        <v>265</v>
+      </c>
+      <c r="AA5" s="91" t="s">
+        <v>266</v>
+      </c>
+      <c r="AB5" s="91" t="s">
+        <v>328</v>
+      </c>
+      <c r="AC5" s="91" t="s">
+        <v>329</v>
+      </c>
+      <c r="AD5" s="91" t="s">
+        <v>330</v>
+      </c>
+      <c r="AE5" s="91" t="s">
+        <v>331</v>
+      </c>
+      <c r="AF5" s="91" t="s">
+        <v>332</v>
+      </c>
+      <c r="AG5" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="AH5" s="91" t="s">
+        <v>268</v>
+      </c>
+      <c r="AI5" s="91" t="s">
+        <v>269</v>
+      </c>
+      <c r="AJ5" s="91" t="s">
+        <v>333</v>
+      </c>
+      <c r="AK5" s="91" t="s">
+        <v>334</v>
+      </c>
+      <c r="AL5" s="91" t="s">
+        <v>270</v>
+      </c>
+      <c r="AM5" s="91" t="s">
+        <v>332</v>
+      </c>
+      <c r="AN5" s="91" t="s">
+        <v>271</v>
+      </c>
+      <c r="AO5" s="91" t="s">
+        <v>272</v>
+      </c>
+      <c r="AP5" s="91" t="s">
+        <v>273</v>
+      </c>
+      <c r="AQ5" s="91" t="s">
+        <v>274</v>
+      </c>
+      <c r="AR5" s="91" t="s">
+        <v>275</v>
+      </c>
+      <c r="AS5" s="91" t="s">
+        <v>276</v>
+      </c>
+      <c r="AT5" s="91" t="s">
+        <v>277</v>
+      </c>
+      <c r="AU5" s="91" t="s">
+        <v>331</v>
+      </c>
+      <c r="AV5" s="91" t="s">
+        <v>278</v>
+      </c>
+      <c r="AW5" s="91" t="s">
+        <v>279</v>
+      </c>
+      <c r="AX5" s="91" t="s">
+        <v>280</v>
+      </c>
+      <c r="AY5" s="91" t="s">
+        <v>281</v>
+      </c>
+      <c r="AZ5" s="91" t="s">
+        <v>282</v>
+      </c>
+      <c r="BA5" s="91" t="s">
+        <v>283</v>
+      </c>
+      <c r="BB5" s="91" t="s">
+        <v>284</v>
+      </c>
+      <c r="BC5" s="91" t="s">
+        <v>285</v>
+      </c>
+      <c r="BD5" s="91" t="s">
+        <v>286</v>
+      </c>
+      <c r="BE5" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="BF5" s="91" t="s">
+        <v>288</v>
+      </c>
+      <c r="BG5" s="91" t="s">
+        <v>335</v>
+      </c>
+      <c r="BH5" s="91" t="s">
+        <v>289</v>
+      </c>
+      <c r="BI5" s="91" t="s">
+        <v>290</v>
+      </c>
+      <c r="BJ5" s="91" t="s">
+        <v>291</v>
+      </c>
+      <c r="BK5" s="91" t="s">
+        <v>292</v>
+      </c>
+      <c r="BL5" s="91" t="s">
+        <v>293</v>
+      </c>
+      <c r="BM5" s="91" t="s">
+        <v>294</v>
+      </c>
+      <c r="BN5" s="91" t="s">
+        <v>295</v>
+      </c>
+      <c r="BO5" s="91" t="s">
+        <v>296</v>
+      </c>
+      <c r="BP5" s="91" t="s">
+        <v>297</v>
+      </c>
+      <c r="BQ5" s="91" t="s">
+        <v>298</v>
+      </c>
+      <c r="BR5" s="91" t="s">
+        <v>299</v>
+      </c>
+      <c r="BS5" s="92"/>
+      <c r="BT5" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="BU5" s="92" t="s">
+        <v>301</v>
+      </c>
+      <c r="BV5" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="BW5" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="BX5" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="BY5" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="BZ5" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="CA5" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="CB5" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="CC5" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="CD5" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="CE5" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="CF5" s="92" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="116"/>
+      <c r="B6" s="117"/>
+      <c r="C6" s="118" t="s">
+        <v>349</v>
+      </c>
+      <c r="D6" s="119" t="s">
+        <v>354</v>
+      </c>
+      <c r="E6" s="119" t="s">
+        <v>356</v>
+      </c>
+      <c r="F6" s="119" t="s">
+        <v>358</v>
+      </c>
+      <c r="G6" s="119" t="s">
+        <v>369</v>
+      </c>
+      <c r="H6" s="119" t="s">
+        <v>374</v>
+      </c>
+      <c r="I6" s="119" t="s">
+        <v>377</v>
+      </c>
+      <c r="J6" s="101" t="s">
+        <v>384</v>
+      </c>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
+      <c r="M6" s="119"/>
+      <c r="N6" s="119"/>
+      <c r="O6" s="119"/>
+      <c r="P6" s="119"/>
+      <c r="Q6" s="119"/>
+      <c r="R6" s="119"/>
+      <c r="S6" s="119"/>
+      <c r="T6" s="119"/>
+      <c r="U6" s="119"/>
+      <c r="V6" s="119"/>
+      <c r="W6" s="119"/>
+      <c r="X6" s="119"/>
+      <c r="Y6" s="119"/>
+      <c r="Z6" s="119"/>
+      <c r="AA6" s="119"/>
+      <c r="AB6" s="119"/>
+      <c r="AC6" s="119"/>
+      <c r="AD6" s="119"/>
+      <c r="AE6" s="119"/>
+      <c r="AF6" s="119"/>
+      <c r="AG6" s="119"/>
+      <c r="AH6" s="119"/>
+      <c r="AI6" s="119"/>
+      <c r="AJ6" s="119"/>
+      <c r="AK6" s="119"/>
+      <c r="AL6" s="119"/>
+      <c r="AM6" s="119"/>
+      <c r="AN6" s="119"/>
+      <c r="AO6" s="119"/>
+      <c r="AP6" s="119"/>
+      <c r="AQ6" s="119"/>
+      <c r="AR6" s="119"/>
+      <c r="AS6" s="119"/>
+      <c r="AT6" s="119"/>
+      <c r="AU6" s="119"/>
+      <c r="AV6" s="119"/>
+      <c r="AW6" s="119"/>
+      <c r="AX6" s="119"/>
+      <c r="AY6" s="119"/>
+      <c r="AZ6" s="119"/>
+      <c r="BA6" s="119"/>
+      <c r="BB6" s="119"/>
+      <c r="BC6" s="119"/>
+      <c r="BD6" s="120"/>
+      <c r="BE6" s="119"/>
+      <c r="BF6" s="119"/>
+      <c r="BG6" s="100" t="s">
+        <v>336</v>
+      </c>
+      <c r="BH6" s="119"/>
+      <c r="BI6" s="119"/>
+      <c r="BJ6" s="119"/>
+      <c r="BK6" s="120"/>
+      <c r="BL6" s="119"/>
+      <c r="BM6" s="119"/>
+      <c r="BN6" s="119"/>
+      <c r="BO6" s="119"/>
+      <c r="BP6" s="119"/>
+      <c r="BQ6" s="119"/>
+      <c r="BR6" s="119"/>
+      <c r="BS6" s="119"/>
+      <c r="BT6" s="119"/>
+      <c r="BU6" s="119"/>
+      <c r="BV6" s="119"/>
+      <c r="BW6" s="119"/>
+      <c r="BX6" s="119"/>
+      <c r="BY6" s="119"/>
+      <c r="BZ6" s="119"/>
+      <c r="CA6" s="119"/>
+      <c r="CB6" s="119"/>
+      <c r="CC6" s="119"/>
+      <c r="CD6" s="119"/>
+      <c r="CE6" s="119"/>
+      <c r="CF6" s="121"/>
+    </row>
+    <row r="7" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="122"/>
+      <c r="B7" s="117"/>
+      <c r="C7" s="123" t="s">
+        <v>350</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F7" s="124" t="s">
+        <v>359</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="J7" s="101" t="s">
+        <v>385</v>
+      </c>
+      <c r="AX7" s="125"/>
+      <c r="AY7" s="125"/>
+      <c r="AZ7" s="125"/>
+      <c r="BA7" s="125"/>
+      <c r="BB7" s="125"/>
+      <c r="BD7" s="126"/>
+      <c r="BG7" s="127"/>
+      <c r="BJ7" s="125"/>
+      <c r="BK7" s="126"/>
+      <c r="CF7" s="128"/>
+    </row>
+    <row r="8" spans="1:84" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="122"/>
+      <c r="B8" s="117"/>
+      <c r="C8" s="123" t="s">
+        <v>351</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="J8" s="101" t="s">
+        <v>386</v>
+      </c>
+      <c r="AX8" s="125"/>
+      <c r="AY8" s="125"/>
+      <c r="AZ8" s="125"/>
+      <c r="BA8" s="125"/>
+      <c r="BB8" s="125"/>
+      <c r="BD8" s="126"/>
+      <c r="BG8" s="127"/>
+      <c r="BJ8" s="125"/>
+      <c r="BK8" s="126"/>
+      <c r="CF8" s="128"/>
+    </row>
+    <row r="9" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="122"/>
+      <c r="B9" s="117"/>
+      <c r="C9" s="123" t="s">
+        <v>352</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="J9" s="101" t="s">
+        <v>387</v>
+      </c>
+      <c r="AX9" s="125"/>
+      <c r="AY9" s="125"/>
+      <c r="AZ9" s="125"/>
+      <c r="BA9" s="125"/>
+      <c r="BB9" s="125"/>
+      <c r="BD9" s="126"/>
+      <c r="BG9" s="127"/>
+      <c r="BJ9" s="125"/>
+      <c r="BK9" s="126"/>
+      <c r="CF9" s="128"/>
+    </row>
+    <row r="10" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="122"/>
+      <c r="B10" s="117"/>
+      <c r="C10" s="123" t="s">
+        <v>353</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="J10" s="101" t="s">
+        <v>388</v>
+      </c>
+      <c r="AX10" s="125"/>
+      <c r="AY10" s="125"/>
+      <c r="AZ10" s="125"/>
+      <c r="BA10" s="125"/>
+      <c r="BB10" s="125"/>
+      <c r="BD10" s="126"/>
+      <c r="BG10" s="127"/>
+      <c r="BJ10" s="125"/>
+      <c r="BK10" s="126"/>
+      <c r="CF10" s="128"/>
+    </row>
+    <row r="11" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="122"/>
+      <c r="B11" s="117"/>
+      <c r="C11" s="123"/>
+      <c r="F11" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="J11" s="101" t="s">
+        <v>389</v>
+      </c>
+      <c r="AX11" s="125"/>
+      <c r="AY11" s="125"/>
+      <c r="AZ11" s="125"/>
+      <c r="BA11" s="125"/>
+      <c r="BB11" s="125"/>
+      <c r="BD11" s="126"/>
+      <c r="BG11" s="127"/>
+      <c r="BJ11" s="125"/>
+      <c r="BK11" s="126"/>
+      <c r="CF11" s="128"/>
+    </row>
+    <row r="12" spans="1:84" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="122"/>
+      <c r="B12" s="117"/>
+      <c r="C12" s="123"/>
+      <c r="F12" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="J12" s="101" t="s">
+        <v>390</v>
+      </c>
+      <c r="AX12" s="125"/>
+      <c r="AY12" s="125"/>
+      <c r="AZ12" s="125"/>
+      <c r="BA12" s="125"/>
+      <c r="BB12" s="125"/>
+      <c r="BD12" s="126"/>
+      <c r="BG12" s="127"/>
+      <c r="BJ12" s="125"/>
+      <c r="BK12" s="126"/>
+      <c r="CF12" s="128"/>
+    </row>
+    <row r="13" spans="1:84" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="122"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="123"/>
+      <c r="J13" s="101" t="s">
+        <v>391</v>
+      </c>
+      <c r="AX13" s="125"/>
+      <c r="AY13" s="125"/>
+      <c r="AZ13" s="125"/>
+      <c r="BA13" s="125"/>
+      <c r="BB13" s="125"/>
+      <c r="BD13" s="126"/>
+      <c r="BG13" s="127"/>
+      <c r="BJ13" s="125"/>
+      <c r="BK13" s="126"/>
+      <c r="CF13" s="128"/>
+    </row>
+    <row r="14" spans="1:84" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="122"/>
+      <c r="B14" s="117"/>
+      <c r="C14" s="123"/>
+      <c r="J14" s="101" t="s">
+        <v>392</v>
+      </c>
+      <c r="AX14" s="125"/>
+      <c r="AY14" s="125"/>
+      <c r="AZ14" s="125"/>
+      <c r="BA14" s="125"/>
+      <c r="BB14" s="125"/>
+      <c r="BD14" s="126"/>
+      <c r="BG14" s="127"/>
+      <c r="BJ14" s="125"/>
+      <c r="BK14" s="126"/>
+      <c r="CF14" s="128"/>
+    </row>
+    <row r="15" spans="1:84" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="129"/>
+      <c r="B15" s="130"/>
+      <c r="C15" s="131"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="132"/>
+      <c r="G15" s="132"/>
+      <c r="H15" s="132"/>
+      <c r="I15" s="132"/>
+      <c r="J15" s="101" t="s">
+        <v>393</v>
+      </c>
+      <c r="K15" s="132"/>
+      <c r="L15" s="132"/>
+      <c r="M15" s="132"/>
+      <c r="N15" s="132"/>
+      <c r="O15" s="132"/>
+      <c r="P15" s="132"/>
+      <c r="Q15" s="132"/>
+      <c r="R15" s="132"/>
+      <c r="S15" s="132"/>
+      <c r="T15" s="132"/>
+      <c r="U15" s="132"/>
+      <c r="V15" s="132"/>
+      <c r="W15" s="132"/>
+      <c r="X15" s="132"/>
+      <c r="Y15" s="132"/>
+      <c r="Z15" s="132"/>
+      <c r="AA15" s="132"/>
+      <c r="AB15" s="132"/>
+      <c r="AC15" s="132"/>
+      <c r="AD15" s="132"/>
+      <c r="AE15" s="132"/>
+      <c r="AF15" s="132"/>
+      <c r="AG15" s="132"/>
+      <c r="AH15" s="132"/>
+      <c r="AI15" s="132"/>
+      <c r="AJ15" s="132"/>
+      <c r="AK15" s="132"/>
+      <c r="AL15" s="132"/>
+      <c r="AM15" s="132"/>
+      <c r="AN15" s="132"/>
+      <c r="AO15" s="132"/>
+      <c r="AP15" s="132"/>
+      <c r="AQ15" s="132"/>
+      <c r="AR15" s="132"/>
+      <c r="AS15" s="132"/>
+      <c r="AT15" s="132"/>
+      <c r="AU15" s="132"/>
+      <c r="AV15" s="132"/>
+      <c r="AW15" s="132"/>
+      <c r="AX15" s="133"/>
+      <c r="AY15" s="133"/>
+      <c r="AZ15" s="133"/>
+      <c r="BA15" s="133"/>
+      <c r="BB15" s="133"/>
+      <c r="BC15" s="132"/>
+      <c r="BD15" s="134"/>
+      <c r="BE15" s="132"/>
+      <c r="BF15" s="132"/>
+      <c r="BG15" s="134"/>
+      <c r="BH15" s="132"/>
+      <c r="BI15" s="132"/>
+      <c r="BJ15" s="133"/>
+      <c r="BK15" s="134"/>
+      <c r="BL15" s="132"/>
+      <c r="BM15" s="132"/>
+      <c r="BN15" s="132"/>
+      <c r="BO15" s="132"/>
+      <c r="BP15" s="132"/>
+      <c r="BQ15" s="132"/>
+      <c r="BR15" s="132"/>
+      <c r="BS15" s="132"/>
+      <c r="BT15" s="132"/>
+      <c r="BU15" s="132"/>
+      <c r="BV15" s="132"/>
+      <c r="BW15" s="132"/>
+      <c r="BX15" s="132"/>
+      <c r="BY15" s="132"/>
+      <c r="BZ15" s="132"/>
+      <c r="CA15" s="132"/>
+      <c r="CB15" s="132"/>
+      <c r="CC15" s="132"/>
+      <c r="CD15" s="132"/>
+      <c r="CE15" s="132"/>
+      <c r="CF15" s="135"/>
+    </row>
+    <row r="16" spans="1:84" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J16" s="101" t="s">
+        <v>394</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:A15"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="BG4" r:id="rId1" xr:uid="{4B5FFA6B-2AB1-46E6-8471-5A507C145283}"/>
+    <hyperlink ref="AT3" r:id="rId2" xr:uid="{5D2D13B3-9C5B-488A-B785-A348C41333BE}"/>
+    <hyperlink ref="AS4" r:id="rId3" xr:uid="{10271E30-10C4-44C6-9BE1-F4068C60AA12}"/>
+    <hyperlink ref="AS3" r:id="rId4" xr:uid="{B40182E7-EACA-40FE-A99E-48AAA775743E}"/>
+    <hyperlink ref="AJ4" r:id="rId5" xr:uid="{17B00242-A3CE-4B96-A734-4513CEE06EF4}"/>
+    <hyperlink ref="AJ3" r:id="rId6" xr:uid="{397F6108-E3C3-4EAF-8EB7-42D1C8071B0E}"/>
+    <hyperlink ref="AD3" r:id="rId7" xr:uid="{CDDFD755-E5FB-4177-9DD3-9BD399EB6441}"/>
+    <hyperlink ref="AD4" r:id="rId8" xr:uid="{3ACD4BC8-A7AF-4395-9920-B41E9BEB9E0F}"/>
+    <hyperlink ref="AC3" r:id="rId9" xr:uid="{A82519EF-C33F-42E4-A6D1-A89E5C4B05EA}"/>
+    <hyperlink ref="AC4" r:id="rId10" xr:uid="{7B06CC04-8C03-4E1B-8131-357897E6AD49}"/>
+    <hyperlink ref="AB4" r:id="rId11" xr:uid="{605B15A7-618E-47C1-AB79-1B963B780B93}"/>
+    <hyperlink ref="AP3" r:id="rId12" xr:uid="{E4659100-C7D5-4193-A864-BB11AA7DB6EE}"/>
+    <hyperlink ref="AN3" r:id="rId13" xr:uid="{DCC65252-59AB-4DBF-AB02-C614A6EDAE4A}"/>
+    <hyperlink ref="AO4" r:id="rId14" xr:uid="{A9A06F6C-9DBE-43A4-A469-0E0ADF7D74FB}"/>
+    <hyperlink ref="AG4" r:id="rId15" xr:uid="{230EE8A6-3C91-47CD-9380-821B5083FAF1}"/>
+    <hyperlink ref="AO3" r:id="rId16" xr:uid="{6DD7848D-53F0-4762-A609-06C383047F37}"/>
+    <hyperlink ref="AI3" r:id="rId17" xr:uid="{1F8B45F8-D17A-41EF-885D-A0748838CA42}"/>
+    <hyperlink ref="AN4" r:id="rId18" xr:uid="{29DA554E-0AF4-4642-AA60-0A6D51EE8421}"/>
+    <hyperlink ref="AL4" r:id="rId19" xr:uid="{B82AF515-DFEA-4FB7-BF80-746681805AE3}"/>
+    <hyperlink ref="AI4" r:id="rId20" xr:uid="{A5C92BB9-8934-4387-834F-1DDA9CF8CF69}"/>
+    <hyperlink ref="X3" r:id="rId21" xr:uid="{372CFCD9-253D-4455-86CA-8835E5AB0623}"/>
+    <hyperlink ref="W3" r:id="rId22" xr:uid="{80DEF454-1716-4E3B-BCC2-495225318598}"/>
+    <hyperlink ref="V3" r:id="rId23" xr:uid="{A27D504E-800E-4540-91C4-75389E69D898}"/>
+    <hyperlink ref="Y4" r:id="rId24" xr:uid="{FCAA888F-11AB-4C5A-989F-7DA718CFBE50}"/>
+    <hyperlink ref="U4" r:id="rId25" xr:uid="{FE1C00C3-0BE4-40D7-9551-CC0C3F8E02F1}"/>
+    <hyperlink ref="U3" r:id="rId26" xr:uid="{42EEF1B8-E61A-4A9D-94B2-DC4E1EE93D39}"/>
+    <hyperlink ref="Z3" r:id="rId27" xr:uid="{A852D345-BE13-44B1-94FE-C4F446707A74}"/>
+    <hyperlink ref="Y3" r:id="rId28" xr:uid="{8BBEE143-3702-44C0-A365-266FBBCF404A}"/>
+    <hyperlink ref="P4" r:id="rId29" xr:uid="{EAA1CA53-A0FC-48CD-9068-41C75F97EC25}"/>
+    <hyperlink ref="P3" r:id="rId30" xr:uid="{C7DA3ED3-450D-40BC-AD3D-E8641BAB7BB5}"/>
+    <hyperlink ref="R3" r:id="rId31" xr:uid="{494915B5-73CA-4DB6-91E3-8B88FD5EDE5B}"/>
+    <hyperlink ref="Q3" r:id="rId32" xr:uid="{148EB626-B321-45DE-9342-2C8619B40BA2}"/>
+    <hyperlink ref="K3" r:id="rId33" xr:uid="{61DBBA85-5D1C-4748-8F37-EBA173304FB5}"/>
+    <hyperlink ref="C3" r:id="rId34" xr:uid="{4920D614-B796-42A6-A61E-F913A26B1037}"/>
+    <hyperlink ref="C4" r:id="rId35" xr:uid="{CC9EF11D-1DAE-4217-80A5-183A5D71A87C}"/>
+    <hyperlink ref="H4" r:id="rId36" xr:uid="{61573CE5-FD70-40F3-9B33-23A08D43A54D}"/>
+    <hyperlink ref="H3" r:id="rId37" xr:uid="{26F61B0D-9101-41EE-A8B5-2D99CB605168}"/>
+    <hyperlink ref="BU4" r:id="rId38" xr:uid="{51316D17-0EA6-40B4-8B66-C4B04172D520}"/>
+    <hyperlink ref="BT4" r:id="rId39" xr:uid="{A3350FCB-102E-45EA-B7CB-C75EB1A759C4}"/>
+    <hyperlink ref="BH4" r:id="rId40" xr:uid="{3114305B-66BA-46CD-817D-6B013C08B14E}"/>
+    <hyperlink ref="D3" r:id="rId41" xr:uid="{3F5F5771-CA82-4869-BF40-BF939DBF29DE}"/>
+    <hyperlink ref="E3" r:id="rId42" xr:uid="{5B41B086-495A-41C1-A384-F42A4DC8CB98}"/>
+    <hyperlink ref="I3" r:id="rId43" xr:uid="{64DD7ED0-3571-4188-864B-1A08421AE3C4}"/>
+    <hyperlink ref="J3" r:id="rId44" xr:uid="{77FD6960-1B0B-4B65-9BFD-6AA61133A07F}"/>
+    <hyperlink ref="J6" r:id="rId45" xr:uid="{B115BC61-6A32-45BA-A08E-C356ED087A53}"/>
+    <hyperlink ref="J7" r:id="rId46" xr:uid="{5BB48EF7-581C-4E06-B980-A9F064E5B24D}"/>
+    <hyperlink ref="J8" r:id="rId47" xr:uid="{04BDB675-1712-4CF6-8E10-6C9CDE5D7B9C}"/>
+    <hyperlink ref="J9" r:id="rId48" xr:uid="{90219696-5F78-466E-9559-83F52A785B62}"/>
+    <hyperlink ref="J10" r:id="rId49" xr:uid="{A3378DCC-2569-4B88-8B54-F9488E8DD526}"/>
+    <hyperlink ref="J11" r:id="rId50" xr:uid="{CB16E9D5-C8FC-4468-B016-E90ED2159B4E}"/>
+    <hyperlink ref="J12" r:id="rId51" xr:uid="{4801F0AB-42D7-4140-9119-984B7FA62EDB}"/>
+    <hyperlink ref="J13" r:id="rId52" xr:uid="{98B26AEB-F06F-4DFD-AEA7-47D2D89921A0}"/>
+    <hyperlink ref="J14" r:id="rId53" xr:uid="{5E90FCB5-D301-463F-B0CC-9509B67F7317}"/>
+    <hyperlink ref="J15" r:id="rId54" xr:uid="{F66B716D-FF1A-470A-8FB3-C49FB6670AAC}"/>
+    <hyperlink ref="J16" r:id="rId55" xr:uid="{8E9ECFCB-B1E1-435F-99E1-C6338EF33DF9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId56"/>
+</worksheet>
 </file>
</xml_diff>